<commit_message>
Updates due to missing owered donuts
</commit_message>
<xml_diff>
--- a/LilDebBracket.xlsx
+++ b/LilDebBracket.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kwiktrip-my.sharepoint.com/personal/am10014003_kwiktrip_com/Documents/Development/lildeb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="8_{BB07369E-1E7E-4ED0-8B1B-ACAC53A5F691}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{46947579-722D-49F5-B64D-D239C0970B3E}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="8_{BB07369E-1E7E-4ED0-8B1B-ACAC53A5F691}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{E8B9B109-3C7A-4310-AE11-506F7DED2E61}"/>
   <bookViews>
     <workbookView xWindow="7860" yWindow="5370" windowWidth="43200" windowHeight="23535" xr2:uid="{10960CD5-A4F3-447E-9C42-3300723A7601}"/>
   </bookViews>
@@ -485,14 +485,14 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="16" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1027,19 +1027,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:12" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="26"/>
     </row>
     <row r="3" spans="1:12" ht="31.5" x14ac:dyDescent="0.5">
       <c r="B3" s="11"/>
@@ -1084,8 +1084,8 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D8" s="26">
-        <v>44664</v>
+      <c r="D8" s="27">
+        <v>44663</v>
       </c>
       <c r="E8" s="18"/>
       <c r="F8" s="15" t="str">
@@ -1095,19 +1095,19 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="16">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B9" s="15" t="str">
         <f>_xlfn.XLOOKUP(Bracket!A9,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
-        <v>Powdered Mini Donuts</v>
-      </c>
-      <c r="D9" s="27"/>
-      <c r="F9" s="26">
+        <v>Chocolate Mini Donuts</v>
+      </c>
+      <c r="D9" s="28"/>
+      <c r="F9" s="27">
         <v>44676</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="26">
+      <c r="B10" s="27">
         <v>44662</v>
       </c>
       <c r="C10" s="18"/>
@@ -1115,7 +1115,7 @@
         <f>_xlfn.XLOOKUP(Bracket!C10,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
         <v>TBD</v>
       </c>
-      <c r="F10" s="26"/>
+      <c r="F10" s="27"/>
       <c r="G10" s="18"/>
       <c r="H10" s="15" t="str">
         <f>_xlfn.XLOOKUP(Bracket!G10,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
@@ -1123,19 +1123,19 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="27"/>
-      <c r="F11" s="26"/>
-      <c r="H11" s="26">
+      <c r="B11" s="28"/>
+      <c r="F11" s="27"/>
+      <c r="H11" s="27">
         <v>44680</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="16">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B12" s="15" t="str">
         <f>_xlfn.XLOOKUP(Bracket!A12,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
-        <v>Chocolate Chip Cream Pies</v>
+        <v>Peanut Butter Crunch</v>
       </c>
       <c r="C12" s="16">
         <v>3</v>
@@ -1144,23 +1144,23 @@
         <f>_xlfn.XLOOKUP(Bracket!C12,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
         <v>Cosmic Brownie</v>
       </c>
-      <c r="F12" s="26"/>
-      <c r="H12" s="26"/>
+      <c r="F12" s="27"/>
+      <c r="H12" s="27"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D13" s="26">
-        <v>44665</v>
+      <c r="D13" s="27">
+        <v>44664</v>
       </c>
       <c r="E13" s="18"/>
       <c r="F13" s="15" t="str">
         <f>_xlfn.XLOOKUP(Bracket!E13,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
         <v>TBD</v>
       </c>
-      <c r="H13" s="26"/>
+      <c r="H13" s="27"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D14" s="27"/>
-      <c r="H14" s="26"/>
+      <c r="D14" s="28"/>
+      <c r="H14" s="27"/>
       <c r="I14" s="18"/>
       <c r="J14" s="15" t="str">
         <f>_xlfn.XLOOKUP(Bracket!I14,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
@@ -1175,14 +1175,14 @@
         <f>_xlfn.XLOOKUP(Bracket!C15,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
         <v>Donut Sticks</v>
       </c>
-      <c r="H15" s="26"/>
-      <c r="J15" s="26">
+      <c r="H15" s="27"/>
+      <c r="J15" s="27">
         <v>44684</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H16" s="26"/>
-      <c r="J16" s="26"/>
+      <c r="H16" s="27"/>
+      <c r="J16" s="27"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C17" s="16">
@@ -1192,28 +1192,28 @@
         <f>_xlfn.XLOOKUP(Bracket!C17,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
         <v>Star Crunch</v>
       </c>
-      <c r="H17" s="26"/>
-      <c r="J17" s="26"/>
+      <c r="H17" s="27"/>
+      <c r="J17" s="27"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D18" s="26">
-        <v>44666</v>
+      <c r="D18" s="27">
+        <v>44665</v>
       </c>
       <c r="E18" s="18"/>
       <c r="F18" s="15" t="str">
         <f>_xlfn.XLOOKUP(Bracket!E18,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
         <v>TBD</v>
       </c>
-      <c r="H18" s="26"/>
-      <c r="J18" s="26"/>
+      <c r="H18" s="27"/>
+      <c r="J18" s="27"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D19" s="27"/>
-      <c r="F19" s="26">
+      <c r="D19" s="28"/>
+      <c r="F19" s="27">
         <v>44677</v>
       </c>
-      <c r="H19" s="26"/>
-      <c r="J19" s="26"/>
+      <c r="H19" s="27"/>
+      <c r="J19" s="27"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C20" s="16">
@@ -1223,17 +1223,17 @@
         <f>_xlfn.XLOOKUP(Bracket!C20,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
         <v>Strawberry Shortcake Rolls</v>
       </c>
-      <c r="F20" s="26"/>
+      <c r="F20" s="27"/>
       <c r="G20" s="18"/>
       <c r="H20" s="15" t="str">
         <f>_xlfn.XLOOKUP(Bracket!G20,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
         <v>TBD</v>
       </c>
-      <c r="J20" s="26"/>
+      <c r="J20" s="27"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F21" s="26"/>
-      <c r="J21" s="26"/>
+      <c r="F21" s="27"/>
+      <c r="J21" s="27"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C22" s="16">
@@ -1243,19 +1243,19 @@
         <f>_xlfn.XLOOKUP(Bracket!C22,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
         <v>Fudge Rounds</v>
       </c>
-      <c r="F22" s="26"/>
-      <c r="J22" s="26"/>
+      <c r="F22" s="27"/>
+      <c r="J22" s="27"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D23" s="26">
-        <v>44669</v>
+      <c r="D23" s="27">
+        <v>44666</v>
       </c>
       <c r="E23" s="18"/>
       <c r="F23" s="15" t="str">
         <f>_xlfn.XLOOKUP(Bracket!E23,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
         <v>TBD</v>
       </c>
-      <c r="J23" s="26"/>
+      <c r="J23" s="27"/>
       <c r="K23" s="18"/>
       <c r="L23" s="15" t="str">
         <f>_xlfn.XLOOKUP(Bracket!K23,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
@@ -1264,8 +1264,8 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B24" s="9"/>
-      <c r="D24" s="27"/>
-      <c r="J24" s="26"/>
+      <c r="D24" s="28"/>
+      <c r="J24" s="27"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B25" s="9"/>
@@ -1276,11 +1276,11 @@
         <f>_xlfn.XLOOKUP(Bracket!C25,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
         <v>Fudge Brownie</v>
       </c>
-      <c r="J25" s="26"/>
+      <c r="J25" s="27"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B26" s="9"/>
-      <c r="J26" s="26"/>
+      <c r="J26" s="27"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B27" s="9"/>
@@ -1291,10 +1291,10 @@
         <f>_xlfn.XLOOKUP(Bracket!C27,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
         <v>Zebra Cakes</v>
       </c>
-      <c r="J27" s="26"/>
+      <c r="J27" s="27"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D28" s="26">
+      <c r="D28" s="27">
         <v>44670</v>
       </c>
       <c r="E28" s="18"/>
@@ -1302,54 +1302,54 @@
         <f>_xlfn.XLOOKUP(Bracket!E28,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
         <v>TBD</v>
       </c>
-      <c r="J28" s="26"/>
+      <c r="J28" s="27"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="16">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B29" s="15" t="str">
         <f>_xlfn.XLOOKUP(Bracket!A29,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
-        <v>Chocolate Mini Donuts</v>
-      </c>
-      <c r="D29" s="27"/>
-      <c r="F29" s="26">
+        <v>Powdered Mini Donuts</v>
+      </c>
+      <c r="D29" s="28"/>
+      <c r="F29" s="27">
         <v>44678</v>
       </c>
-      <c r="J29" s="26"/>
+      <c r="J29" s="27"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B30" s="26">
-        <v>44663</v>
+      <c r="B30" s="27">
+        <v>44669</v>
       </c>
       <c r="C30" s="18"/>
       <c r="D30" s="15" t="str">
         <f>_xlfn.XLOOKUP(Bracket!C30,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
         <v>TBD</v>
       </c>
-      <c r="F30" s="26"/>
+      <c r="F30" s="27"/>
       <c r="G30" s="18"/>
       <c r="H30" s="15" t="str">
         <f>_xlfn.XLOOKUP(Bracket!G30,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
         <v>TBD</v>
       </c>
-      <c r="J30" s="26"/>
+      <c r="J30" s="27"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B31" s="27"/>
-      <c r="F31" s="26"/>
-      <c r="H31" s="26">
+      <c r="B31" s="28"/>
+      <c r="F31" s="27"/>
+      <c r="H31" s="27">
         <v>44683</v>
       </c>
-      <c r="J31" s="26"/>
+      <c r="J31" s="27"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="16">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B32" s="15" t="str">
         <f>_xlfn.XLOOKUP(Bracket!A32,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
-        <v>Peanut Butter Crunch</v>
+        <v>Chocolate Chip Cream Pies</v>
       </c>
       <c r="C32" s="16">
         <v>4</v>
@@ -1358,12 +1358,12 @@
         <f>_xlfn.XLOOKUP(Bracket!C32,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
         <v>Nutty Buddy</v>
       </c>
-      <c r="F32" s="26"/>
-      <c r="H32" s="26"/>
-      <c r="J32" s="26"/>
+      <c r="F32" s="27"/>
+      <c r="H32" s="27"/>
+      <c r="J32" s="27"/>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D33" s="26">
+      <c r="D33" s="27">
         <v>44671</v>
       </c>
       <c r="E33" s="18"/>
@@ -1371,12 +1371,12 @@
         <f>_xlfn.XLOOKUP(Bracket!E33,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
         <v>TBD</v>
       </c>
-      <c r="H33" s="26"/>
-      <c r="J33" s="26"/>
+      <c r="H33" s="27"/>
+      <c r="J33" s="27"/>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D34" s="27"/>
-      <c r="H34" s="26"/>
+      <c r="D34" s="28"/>
+      <c r="H34" s="27"/>
       <c r="I34" s="18"/>
       <c r="J34" s="15" t="str">
         <f>_xlfn.XLOOKUP(Bracket!I34,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
@@ -1391,10 +1391,10 @@
         <f>_xlfn.XLOOKUP(Bracket!C35,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
         <v>Honey Buns</v>
       </c>
-      <c r="H35" s="26"/>
+      <c r="H35" s="27"/>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="H36" s="26"/>
+      <c r="H36" s="27"/>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C37" s="16">
@@ -1404,10 +1404,10 @@
         <f>_xlfn.XLOOKUP(Bracket!C37,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
         <v>Oatmeal Cream Pies</v>
       </c>
-      <c r="H37" s="26"/>
+      <c r="H37" s="27"/>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D38" s="26">
+      <c r="D38" s="27">
         <v>44672</v>
       </c>
       <c r="E38" s="18"/>
@@ -1415,14 +1415,14 @@
         <f>_xlfn.XLOOKUP(Bracket!E38,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
         <v>TBD</v>
       </c>
-      <c r="H38" s="26"/>
+      <c r="H38" s="27"/>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D39" s="27"/>
-      <c r="F39" s="26">
+      <c r="D39" s="28"/>
+      <c r="F39" s="27">
         <v>44679</v>
       </c>
-      <c r="H39" s="26"/>
+      <c r="H39" s="27"/>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C40" s="16">
@@ -1432,7 +1432,7 @@
         <f>_xlfn.XLOOKUP(Bracket!C40,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
         <v>Birthday Cakes</v>
       </c>
-      <c r="F40" s="26"/>
+      <c r="F40" s="27"/>
       <c r="G40" s="18"/>
       <c r="H40" s="15" t="str">
         <f>_xlfn.XLOOKUP(Bracket!G40,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
@@ -1440,7 +1440,7 @@
       </c>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F41" s="26"/>
+      <c r="F41" s="27"/>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C42" s="16">
@@ -1450,10 +1450,10 @@
         <f>_xlfn.XLOOKUP(Bracket!C42,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
         <v>Fancy Cakes</v>
       </c>
-      <c r="F42" s="26"/>
+      <c r="F42" s="27"/>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D43" s="26">
+      <c r="D43" s="27">
         <v>44673</v>
       </c>
       <c r="E43" s="18"/>
@@ -1464,7 +1464,7 @@
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B44" s="9"/>
-      <c r="D44" s="27"/>
+      <c r="D44" s="28"/>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B45" s="9"/>
@@ -1484,17 +1484,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B2:L2"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="H11:H19"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="F9:F12"/>
-    <mergeCell ref="F19:F22"/>
-    <mergeCell ref="F29:F32"/>
-    <mergeCell ref="F39:F42"/>
     <mergeCell ref="H31:H39"/>
     <mergeCell ref="J15:J33"/>
     <mergeCell ref="B10:B11"/>
@@ -1502,6 +1491,17 @@
     <mergeCell ref="D28:D29"/>
     <mergeCell ref="D33:D34"/>
     <mergeCell ref="D38:D39"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="F9:F12"/>
+    <mergeCell ref="F19:F22"/>
+    <mergeCell ref="F29:F32"/>
+    <mergeCell ref="F39:F42"/>
+    <mergeCell ref="B2:L2"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="H11:H19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updates to spreadsheet formatting
</commit_message>
<xml_diff>
--- a/LilDebBracket.xlsx
+++ b/LilDebBracket.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kwiktrip-my.sharepoint.com/personal/am10014003_kwiktrip_com/Documents/Development/lildeb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="143" documentId="8_{BB07369E-1E7E-4ED0-8B1B-ACAC53A5F691}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{A48958E1-4A9D-440A-BCDA-2F3D5A9276FE}"/>
+  <xr:revisionPtr revIDLastSave="174" documentId="8_{BB07369E-1E7E-4ED0-8B1B-ACAC53A5F691}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F243CD5C-9170-4359-98D3-2AEFB7C7A019}"/>
   <bookViews>
     <workbookView xWindow="19185" yWindow="15900" windowWidth="19200" windowHeight="15900" xr2:uid="{10960CD5-A4F3-447E-9C42-3300723A7601}"/>
   </bookViews>
@@ -189,7 +189,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -228,16 +228,42 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="24">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -506,11 +532,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -559,52 +622,42 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="4" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="4" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="4" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="4" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="4" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="4" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="4" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="4" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="4" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="13">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -749,6 +802,26 @@
         <scheme val="minor"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -763,37 +836,37 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DED839B5-A689-44EC-B2B9-CD5382E40C0F}" name="Table1" displayName="Table1" ref="A1:I31" totalsRowShown="0" headerRowDxfId="12" headerRowBorderDxfId="11" tableBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DED839B5-A689-44EC-B2B9-CD5382E40C0F}" name="Table1" displayName="Table1" ref="A1:I31" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8">
   <autoFilter ref="A1:I31" xr:uid="{DED839B5-A689-44EC-B2B9-CD5382E40C0F}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I31">
     <sortCondition ref="I1:I31"/>
   </sortState>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{33A657BA-C124-40E7-9776-39E26BAD0A73}" name="Product"/>
-    <tableColumn id="2" xr3:uid="{7A5E4489-9425-4066-9BAC-CF29C2B4F92B}" name="Michael" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{7A5E4489-9425-4066-9BAC-CF29C2B4F92B}" name="Michael" dataDxfId="7"/>
     <tableColumn id="3" xr3:uid="{3229F806-5483-4632-BDF7-25835E56C95D}" name="Steph"/>
     <tableColumn id="4" xr3:uid="{9DC657F1-8F27-4B04-A113-8E816CF72F42}" name="Megan"/>
     <tableColumn id="5" xr3:uid="{5073D592-7FBA-49AA-AA57-BB4A74795419}" name="Bill"/>
     <tableColumn id="6" xr3:uid="{2725D0F3-8C6D-4B1F-9C50-DEB1777A9F7C}" name="Austin"/>
     <tableColumn id="7" xr3:uid="{728A598D-CDAD-430F-91BC-099D4B675146}" name="Katrina"/>
-    <tableColumn id="8" xr3:uid="{6556397C-4851-419F-8D9E-A9416EF14135}" name="Votes" dataDxfId="8">
+    <tableColumn id="8" xr3:uid="{6556397C-4851-419F-8D9E-A9416EF14135}" name="Votes" dataDxfId="6">
       <calculatedColumnFormula>COUNTA(B2:G2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{0AB69B5C-AA2C-4700-93A6-08909EDD760F}" name="Seed" dataDxfId="7"/>
+    <tableColumn id="9" xr3:uid="{0AB69B5C-AA2C-4700-93A6-08909EDD760F}" name="Seed" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8FF0ED2D-5058-4F61-8176-3805AD9FA9A1}" name="Table2" displayName="Table2" ref="A1:B19" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8FF0ED2D-5058-4F61-8176-3805AD9FA9A1}" name="Table2" displayName="Table2" ref="A1:B19" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="3" tableBorderDxfId="2">
   <autoFilter ref="A1:B19" xr:uid="{992AE444-750B-4121-820A-6F9D8D7D5FA7}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B19">
     <sortCondition ref="B1:B19"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{88D4C9A0-10CD-48F6-AD6D-8DA7DD6D397B}" name="Product" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{1D5D0DF5-A7D7-4613-932C-887FEE531C0B}" name="Who's buyin'?" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{88D4C9A0-10CD-48F6-AD6D-8DA7DD6D397B}" name="Product" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{1D5D0DF5-A7D7-4613-932C-887FEE531C0B}" name="Who's buyin'?" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1096,7 +1169,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0E5BB06-8011-4308-BEC9-9A7436B98035}">
-  <dimension ref="A2:Q47"/>
+  <dimension ref="A1:Q47"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1117,27 +1190,28 @@
     <col min="17" max="17" width="7.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:17" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="B2" s="33" t="s">
+    <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:17" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B2" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="33"/>
-    </row>
-    <row r="3" spans="1:17" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="41"/>
+      <c r="N2" s="41"/>
+      <c r="O2" s="41"/>
+      <c r="P2" s="41"/>
+      <c r="Q2" s="42"/>
+    </row>
+    <row r="3" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B3" s="11"/>
       <c r="C3" s="26"/>
       <c r="D3" s="11"/>
@@ -1191,10 +1265,10 @@
       <c r="F7" s="27"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E8" s="31">
+      <c r="E8" s="34">
         <v>44663</v>
       </c>
-      <c r="F8" s="34"/>
+      <c r="F8" s="35"/>
       <c r="G8" s="18"/>
       <c r="H8" s="15" t="str">
         <f>_xlfn.XLOOKUP(Bracket!G8,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
@@ -1206,25 +1280,25 @@
       <c r="A9" s="16">
         <v>16</v>
       </c>
-      <c r="B9" s="15" t="str">
+      <c r="B9" s="33" t="str">
         <f>_xlfn.XLOOKUP(Bracket!A9,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
         <v>Chocolate Mini Donuts</v>
       </c>
-      <c r="C9" s="27">
+      <c r="C9" s="32">
         <v>2</v>
       </c>
-      <c r="E9" s="32"/>
-      <c r="F9" s="35"/>
-      <c r="H9" s="31">
+      <c r="E9" s="36"/>
+      <c r="F9" s="37"/>
+      <c r="H9" s="34">
         <v>44677</v>
       </c>
-      <c r="I9" s="34"/>
+      <c r="I9" s="35"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B10" s="31">
+      <c r="B10" s="34">
         <v>44662</v>
       </c>
-      <c r="C10" s="34"/>
+      <c r="C10" s="35"/>
       <c r="D10" s="18">
         <v>17</v>
       </c>
@@ -1233,8 +1307,8 @@
         <v>Peanut Butter Crunch</v>
       </c>
       <c r="F10" s="28"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="36"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="39"/>
       <c r="J10" s="18"/>
       <c r="K10" s="15" t="str">
         <f>_xlfn.XLOOKUP(Bracket!J10,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
@@ -1243,24 +1317,24 @@
       <c r="L10" s="27"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B11" s="32"/>
-      <c r="C11" s="35"/>
-      <c r="H11" s="30"/>
-      <c r="I11" s="36"/>
-      <c r="K11" s="31">
+      <c r="B11" s="36"/>
+      <c r="C11" s="37"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="39"/>
+      <c r="K11" s="34">
         <v>44683</v>
       </c>
-      <c r="L11" s="34"/>
+      <c r="L11" s="35"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="16">
         <v>17</v>
       </c>
-      <c r="B12" s="15" t="str">
+      <c r="B12" s="30" t="str">
         <f>_xlfn.XLOOKUP(Bracket!A12,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
         <v>Peanut Butter Crunch</v>
       </c>
-      <c r="C12" s="28">
+      <c r="C12" s="31">
         <v>6</v>
       </c>
       <c r="D12" s="16">
@@ -1271,30 +1345,30 @@
         <v>Cosmic Brownie</v>
       </c>
       <c r="F12" s="27"/>
-      <c r="H12" s="32"/>
-      <c r="I12" s="35"/>
-      <c r="K12" s="30"/>
-      <c r="L12" s="36"/>
+      <c r="H12" s="36"/>
+      <c r="I12" s="37"/>
+      <c r="K12" s="38"/>
+      <c r="L12" s="39"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E13" s="31">
+      <c r="E13" s="34">
         <v>44664</v>
       </c>
-      <c r="F13" s="34"/>
+      <c r="F13" s="35"/>
       <c r="G13" s="18"/>
       <c r="H13" s="15" t="str">
         <f>_xlfn.XLOOKUP(Bracket!G13,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
         <v>TBD</v>
       </c>
       <c r="I13" s="28"/>
-      <c r="K13" s="30"/>
-      <c r="L13" s="36"/>
+      <c r="K13" s="38"/>
+      <c r="L13" s="39"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E14" s="32"/>
-      <c r="F14" s="35"/>
-      <c r="K14" s="30"/>
-      <c r="L14" s="36"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="37"/>
+      <c r="K14" s="38"/>
+      <c r="L14" s="39"/>
       <c r="M14" s="18"/>
       <c r="N14" s="15" t="str">
         <f>_xlfn.XLOOKUP(Bracket!M14,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
@@ -1311,18 +1385,18 @@
         <v>Donut Sticks</v>
       </c>
       <c r="F15" s="28"/>
-      <c r="K15" s="30"/>
-      <c r="L15" s="36"/>
-      <c r="N15" s="31">
+      <c r="K15" s="38"/>
+      <c r="L15" s="39"/>
+      <c r="N15" s="34">
         <v>44685</v>
       </c>
-      <c r="O15" s="34"/>
+      <c r="O15" s="35"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="K16" s="30"/>
-      <c r="L16" s="36"/>
-      <c r="N16" s="30"/>
-      <c r="O16" s="36"/>
+      <c r="K16" s="38"/>
+      <c r="L16" s="39"/>
+      <c r="N16" s="38"/>
+      <c r="O16" s="39"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D17" s="16">
@@ -1333,38 +1407,38 @@
         <v>Star Crunch</v>
       </c>
       <c r="F17" s="27"/>
-      <c r="K17" s="30"/>
-      <c r="L17" s="36"/>
-      <c r="N17" s="30"/>
-      <c r="O17" s="36"/>
+      <c r="K17" s="38"/>
+      <c r="L17" s="39"/>
+      <c r="N17" s="38"/>
+      <c r="O17" s="39"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E18" s="31">
+      <c r="E18" s="34">
         <v>44665</v>
       </c>
-      <c r="F18" s="34"/>
+      <c r="F18" s="35"/>
       <c r="G18" s="18"/>
       <c r="H18" s="15" t="str">
         <f>_xlfn.XLOOKUP(Bracket!G18,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
         <v>TBD</v>
       </c>
       <c r="I18" s="27"/>
-      <c r="K18" s="30"/>
-      <c r="L18" s="36"/>
-      <c r="N18" s="30"/>
-      <c r="O18" s="36"/>
+      <c r="K18" s="38"/>
+      <c r="L18" s="39"/>
+      <c r="N18" s="38"/>
+      <c r="O18" s="39"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E19" s="32"/>
-      <c r="F19" s="35"/>
-      <c r="H19" s="31">
+      <c r="E19" s="36"/>
+      <c r="F19" s="37"/>
+      <c r="H19" s="34">
         <v>44678</v>
       </c>
-      <c r="I19" s="34"/>
-      <c r="K19" s="32"/>
-      <c r="L19" s="35"/>
-      <c r="N19" s="30"/>
-      <c r="O19" s="36"/>
+      <c r="I19" s="35"/>
+      <c r="K19" s="36"/>
+      <c r="L19" s="37"/>
+      <c r="N19" s="38"/>
+      <c r="O19" s="39"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D20" s="16">
@@ -1375,22 +1449,22 @@
         <v>Strawberry Shortcake Rolls</v>
       </c>
       <c r="F20" s="28"/>
-      <c r="H20" s="30"/>
-      <c r="I20" s="36"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="39"/>
       <c r="J20" s="18"/>
       <c r="K20" s="15" t="str">
         <f>_xlfn.XLOOKUP(Bracket!J20,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
         <v>TBD</v>
       </c>
       <c r="L20" s="28"/>
-      <c r="N20" s="30"/>
-      <c r="O20" s="36"/>
+      <c r="N20" s="38"/>
+      <c r="O20" s="39"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="H21" s="30"/>
-      <c r="I21" s="36"/>
-      <c r="N21" s="30"/>
-      <c r="O21" s="36"/>
+      <c r="H21" s="38"/>
+      <c r="I21" s="39"/>
+      <c r="N21" s="38"/>
+      <c r="O21" s="39"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D22" s="16">
@@ -1401,24 +1475,24 @@
         <v>Fudge Rounds</v>
       </c>
       <c r="F22" s="27"/>
-      <c r="H22" s="32"/>
-      <c r="I22" s="35"/>
-      <c r="N22" s="30"/>
-      <c r="O22" s="36"/>
+      <c r="H22" s="36"/>
+      <c r="I22" s="37"/>
+      <c r="N22" s="38"/>
+      <c r="O22" s="39"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E23" s="31">
+      <c r="E23" s="34">
         <v>44669</v>
       </c>
-      <c r="F23" s="34"/>
+      <c r="F23" s="35"/>
       <c r="G23" s="18"/>
       <c r="H23" s="15" t="str">
         <f>_xlfn.XLOOKUP(Bracket!G23,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
         <v>TBD</v>
       </c>
       <c r="I23" s="28"/>
-      <c r="N23" s="30"/>
-      <c r="O23" s="36"/>
+      <c r="N23" s="38"/>
+      <c r="O23" s="39"/>
       <c r="P23" s="18"/>
       <c r="Q23" s="15" t="str">
         <f>_xlfn.XLOOKUP(Bracket!P23,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
@@ -1428,10 +1502,10 @@
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
-      <c r="E24" s="32"/>
-      <c r="F24" s="35"/>
-      <c r="N24" s="30"/>
-      <c r="O24" s="36"/>
+      <c r="E24" s="36"/>
+      <c r="F24" s="37"/>
+      <c r="N24" s="38"/>
+      <c r="O24" s="39"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B25" s="9"/>
@@ -1444,14 +1518,14 @@
         <v>Fudge Brownie</v>
       </c>
       <c r="F25" s="28"/>
-      <c r="N25" s="30"/>
-      <c r="O25" s="36"/>
+      <c r="N25" s="38"/>
+      <c r="O25" s="39"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
-      <c r="N26" s="30"/>
-      <c r="O26" s="36"/>
+      <c r="N26" s="38"/>
+      <c r="O26" s="39"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B27" s="9"/>
@@ -1464,22 +1538,22 @@
         <v>Zebra Cakes</v>
       </c>
       <c r="F27" s="27"/>
-      <c r="N27" s="30"/>
-      <c r="O27" s="36"/>
+      <c r="N27" s="38"/>
+      <c r="O27" s="39"/>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E28" s="31">
+      <c r="E28" s="34">
         <v>44671</v>
       </c>
-      <c r="F28" s="34"/>
+      <c r="F28" s="35"/>
       <c r="G28" s="18"/>
       <c r="H28" s="15" t="str">
         <f>_xlfn.XLOOKUP(Bracket!G28,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
         <v>TBD</v>
       </c>
       <c r="I28" s="27"/>
-      <c r="N28" s="30"/>
-      <c r="O28" s="36"/>
+      <c r="N28" s="38"/>
+      <c r="O28" s="39"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="16">
@@ -1490,48 +1564,48 @@
         <v>Powdered Mini Donuts</v>
       </c>
       <c r="C29" s="27"/>
-      <c r="E29" s="32"/>
-      <c r="F29" s="35"/>
-      <c r="H29" s="31">
+      <c r="E29" s="36"/>
+      <c r="F29" s="37"/>
+      <c r="H29" s="34">
         <v>44679</v>
       </c>
-      <c r="I29" s="34"/>
-      <c r="N29" s="30"/>
-      <c r="O29" s="36"/>
+      <c r="I29" s="35"/>
+      <c r="N29" s="38"/>
+      <c r="O29" s="39"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B30" s="31">
+      <c r="B30" s="34">
         <v>44670</v>
       </c>
-      <c r="C30" s="34"/>
+      <c r="C30" s="35"/>
       <c r="D30" s="18"/>
       <c r="E30" s="15" t="str">
         <f>_xlfn.XLOOKUP(Bracket!D30,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
         <v>TBD</v>
       </c>
       <c r="F30" s="28"/>
-      <c r="H30" s="30"/>
-      <c r="I30" s="36"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="39"/>
       <c r="J30" s="18"/>
       <c r="K30" s="15" t="str">
         <f>_xlfn.XLOOKUP(Bracket!J30,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
         <v>TBD</v>
       </c>
       <c r="L30" s="27"/>
-      <c r="N30" s="30"/>
-      <c r="O30" s="36"/>
+      <c r="N30" s="38"/>
+      <c r="O30" s="39"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B31" s="32"/>
-      <c r="C31" s="35"/>
-      <c r="H31" s="30"/>
-      <c r="I31" s="36"/>
-      <c r="K31" s="31">
+      <c r="B31" s="36"/>
+      <c r="C31" s="37"/>
+      <c r="H31" s="38"/>
+      <c r="I31" s="39"/>
+      <c r="K31" s="34">
         <v>44684</v>
       </c>
-      <c r="L31" s="34"/>
-      <c r="N31" s="30"/>
-      <c r="O31" s="36"/>
+      <c r="L31" s="35"/>
+      <c r="N31" s="38"/>
+      <c r="O31" s="39"/>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="16">
@@ -1550,34 +1624,34 @@
         <v>Nutty Buddy</v>
       </c>
       <c r="F32" s="27"/>
-      <c r="H32" s="32"/>
-      <c r="I32" s="35"/>
-      <c r="K32" s="30"/>
-      <c r="L32" s="36"/>
-      <c r="N32" s="30"/>
-      <c r="O32" s="36"/>
+      <c r="H32" s="36"/>
+      <c r="I32" s="37"/>
+      <c r="K32" s="38"/>
+      <c r="L32" s="39"/>
+      <c r="N32" s="38"/>
+      <c r="O32" s="39"/>
     </row>
     <row r="33" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="E33" s="31">
+      <c r="E33" s="34">
         <v>44672</v>
       </c>
-      <c r="F33" s="34"/>
+      <c r="F33" s="35"/>
       <c r="G33" s="18"/>
       <c r="H33" s="15" t="str">
         <f>_xlfn.XLOOKUP(Bracket!G33,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
         <v>TBD</v>
       </c>
       <c r="I33" s="28"/>
-      <c r="K33" s="30"/>
-      <c r="L33" s="36"/>
-      <c r="N33" s="32"/>
-      <c r="O33" s="35"/>
+      <c r="K33" s="38"/>
+      <c r="L33" s="39"/>
+      <c r="N33" s="36"/>
+      <c r="O33" s="37"/>
     </row>
     <row r="34" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="E34" s="32"/>
-      <c r="F34" s="35"/>
-      <c r="K34" s="30"/>
-      <c r="L34" s="36"/>
+      <c r="E34" s="36"/>
+      <c r="F34" s="37"/>
+      <c r="K34" s="38"/>
+      <c r="L34" s="39"/>
       <c r="M34" s="18"/>
       <c r="N34" s="15" t="str">
         <f>_xlfn.XLOOKUP(Bracket!M34,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
@@ -1594,12 +1668,12 @@
         <v>Honey Buns</v>
       </c>
       <c r="F35" s="28"/>
-      <c r="K35" s="30"/>
-      <c r="L35" s="36"/>
+      <c r="K35" s="38"/>
+      <c r="L35" s="39"/>
     </row>
     <row r="36" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="K36" s="30"/>
-      <c r="L36" s="36"/>
+      <c r="K36" s="38"/>
+      <c r="L36" s="39"/>
     </row>
     <row r="37" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D37" s="16">
@@ -1610,32 +1684,32 @@
         <v>Oatmeal Cream Pies</v>
       </c>
       <c r="F37" s="27"/>
-      <c r="K37" s="30"/>
-      <c r="L37" s="36"/>
+      <c r="K37" s="38"/>
+      <c r="L37" s="39"/>
     </row>
     <row r="38" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="E38" s="31">
+      <c r="E38" s="34">
         <v>44673</v>
       </c>
-      <c r="F38" s="34"/>
+      <c r="F38" s="35"/>
       <c r="G38" s="18"/>
       <c r="H38" s="15" t="str">
         <f>_xlfn.XLOOKUP(Bracket!G38,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
         <v>TBD</v>
       </c>
       <c r="I38" s="27"/>
-      <c r="K38" s="30"/>
-      <c r="L38" s="36"/>
+      <c r="K38" s="38"/>
+      <c r="L38" s="39"/>
     </row>
     <row r="39" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="E39" s="32"/>
-      <c r="F39" s="35"/>
-      <c r="H39" s="31">
+      <c r="E39" s="36"/>
+      <c r="F39" s="37"/>
+      <c r="H39" s="34">
         <v>44680</v>
       </c>
-      <c r="I39" s="34"/>
-      <c r="K39" s="32"/>
-      <c r="L39" s="35"/>
+      <c r="I39" s="35"/>
+      <c r="K39" s="36"/>
+      <c r="L39" s="37"/>
     </row>
     <row r="40" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D40" s="16">
@@ -1646,8 +1720,8 @@
         <v>Birthday Cakes</v>
       </c>
       <c r="F40" s="28"/>
-      <c r="H40" s="30"/>
-      <c r="I40" s="36"/>
+      <c r="H40" s="38"/>
+      <c r="I40" s="39"/>
       <c r="J40" s="18"/>
       <c r="K40" s="15" t="str">
         <f>_xlfn.XLOOKUP(Bracket!J40,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
@@ -1656,8 +1730,8 @@
       <c r="L40" s="28"/>
     </row>
     <row r="41" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="H41" s="30"/>
-      <c r="I41" s="36"/>
+      <c r="H41" s="38"/>
+      <c r="I41" s="39"/>
     </row>
     <row r="42" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D42" s="16">
@@ -1668,14 +1742,14 @@
         <v>Fancy Cakes</v>
       </c>
       <c r="F42" s="27"/>
-      <c r="H42" s="32"/>
-      <c r="I42" s="35"/>
+      <c r="H42" s="36"/>
+      <c r="I42" s="37"/>
     </row>
     <row r="43" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="E43" s="31">
+      <c r="E43" s="34">
         <v>44676</v>
       </c>
-      <c r="F43" s="34"/>
+      <c r="F43" s="35"/>
       <c r="G43" s="18"/>
       <c r="H43" s="15" t="str">
         <f>_xlfn.XLOOKUP(Bracket!G43,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
@@ -1686,8 +1760,8 @@
     <row r="44" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B44" s="9"/>
       <c r="C44" s="9"/>
-      <c r="E44" s="32"/>
-      <c r="F44" s="35"/>
+      <c r="E44" s="36"/>
+      <c r="F44" s="37"/>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45" s="9"/>
@@ -1711,11 +1785,11 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B2:Q2"/>
-    <mergeCell ref="B10:C11"/>
-    <mergeCell ref="E8:F9"/>
-    <mergeCell ref="E13:F14"/>
-    <mergeCell ref="E18:F19"/>
+    <mergeCell ref="E38:F39"/>
+    <mergeCell ref="E43:F44"/>
+    <mergeCell ref="H29:I32"/>
+    <mergeCell ref="H39:I42"/>
+    <mergeCell ref="B30:C31"/>
     <mergeCell ref="E23:F24"/>
     <mergeCell ref="H9:I12"/>
     <mergeCell ref="H19:I22"/>
@@ -1723,12 +1797,12 @@
     <mergeCell ref="N15:O33"/>
     <mergeCell ref="E28:F29"/>
     <mergeCell ref="E33:F34"/>
-    <mergeCell ref="E38:F39"/>
-    <mergeCell ref="E43:F44"/>
-    <mergeCell ref="H29:I32"/>
-    <mergeCell ref="H39:I42"/>
-    <mergeCell ref="B30:C31"/>
     <mergeCell ref="K31:L39"/>
+    <mergeCell ref="B2:Q2"/>
+    <mergeCell ref="B10:C11"/>
+    <mergeCell ref="E8:F9"/>
+    <mergeCell ref="E13:F14"/>
+    <mergeCell ref="E18:F19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2450,10 +2524,10 @@
     <sortCondition ref="A2:A31"/>
   </sortState>
   <conditionalFormatting sqref="H2:H31">
-    <cfRule type="top10" dxfId="1" priority="2" rank="16"/>
+    <cfRule type="top10" dxfId="12" priority="2" rank="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B32:G32">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>16</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
4/28 - Double Elimination!
</commit_message>
<xml_diff>
--- a/LilDebBracket.xlsx
+++ b/LilDebBracket.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdd45780\Documents\GitHub\lildeb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87C45BC2-9A57-40DA-BC3A-8727F75AEFF1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDA87C47-B3DF-480C-85B5-8B478F21A855}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="28800" windowHeight="15600" xr2:uid="{10960CD5-A4F3-447E-9C42-3300723A7601}"/>
+    <workbookView xWindow="-35730" yWindow="14730" windowWidth="43200" windowHeight="23535" xr2:uid="{10960CD5-A4F3-447E-9C42-3300723A7601}"/>
   </bookViews>
   <sheets>
     <sheet name="Bracket" sheetId="3" r:id="rId1"/>
@@ -633,6 +633,15 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="16" fontId="4" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -650,15 +659,6 @@
     </xf>
     <xf numFmtId="16" fontId="4" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1179,7 +1179,7 @@
   <dimension ref="A1:Q47"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1192,7 +1192,7 @@
     <col min="6" max="6" width="3.7109375" customWidth="1"/>
     <col min="8" max="8" width="25" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="3.7109375" customWidth="1"/>
-    <col min="11" max="11" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="3.7109375" customWidth="1"/>
     <col min="14" max="14" width="14" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="3.7109375" customWidth="1"/>
@@ -1201,24 +1201,24 @@
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:17" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="45"/>
-      <c r="M2" s="45"/>
-      <c r="N2" s="45"/>
-      <c r="O2" s="45"/>
-      <c r="P2" s="45"/>
-      <c r="Q2" s="46"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
+      <c r="N2" s="39"/>
+      <c r="O2" s="39"/>
+      <c r="P2" s="39"/>
+      <c r="Q2" s="40"/>
     </row>
     <row r="3" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B3" s="11"/>
@@ -1276,18 +1276,20 @@
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E8" s="38">
+      <c r="E8" s="41">
         <v>44663</v>
       </c>
-      <c r="F8" s="39"/>
+      <c r="F8" s="42"/>
       <c r="G8" s="18">
         <v>17</v>
       </c>
-      <c r="H8" s="15" t="str">
+      <c r="H8" s="30" t="str">
         <f>_xlfn.XLOOKUP(Bracket!G8,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
         <v>Peanut Butter Crunch</v>
       </c>
-      <c r="I8" s="27"/>
+      <c r="I8" s="30">
+        <v>5</v>
+      </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="16">
@@ -1300,18 +1302,18 @@
       <c r="C9" s="32">
         <v>2</v>
       </c>
-      <c r="E9" s="40"/>
-      <c r="F9" s="41"/>
-      <c r="H9" s="38">
-        <v>44678</v>
-      </c>
-      <c r="I9" s="39"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="44"/>
+      <c r="H9" s="41">
+        <v>44679</v>
+      </c>
+      <c r="I9" s="42"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B10" s="38">
+      <c r="B10" s="41">
         <v>44662</v>
       </c>
-      <c r="C10" s="39"/>
+      <c r="C10" s="42"/>
       <c r="D10" s="18">
         <v>17</v>
       </c>
@@ -1322,24 +1324,26 @@
       <c r="F10" s="31">
         <v>4</v>
       </c>
-      <c r="H10" s="42"/>
-      <c r="I10" s="43"/>
-      <c r="J10" s="18"/>
+      <c r="H10" s="45"/>
+      <c r="I10" s="46"/>
+      <c r="J10" s="18">
+        <v>17</v>
+      </c>
       <c r="K10" s="15" t="str">
         <f>_xlfn.XLOOKUP(Bracket!J10,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
-        <v>TBD</v>
+        <v>Peanut Butter Crunch</v>
       </c>
       <c r="L10" s="27"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B11" s="40"/>
-      <c r="C11" s="41"/>
-      <c r="H11" s="42"/>
-      <c r="I11" s="43"/>
-      <c r="K11" s="38">
+      <c r="B11" s="43"/>
+      <c r="C11" s="44"/>
+      <c r="H11" s="45"/>
+      <c r="I11" s="46"/>
+      <c r="K11" s="41">
         <v>44683</v>
       </c>
-      <c r="L11" s="39"/>
+      <c r="L11" s="42"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="16">
@@ -1362,32 +1366,34 @@
       <c r="F12" s="34">
         <v>3</v>
       </c>
-      <c r="H12" s="40"/>
-      <c r="I12" s="41"/>
-      <c r="K12" s="42"/>
-      <c r="L12" s="43"/>
+      <c r="H12" s="43"/>
+      <c r="I12" s="44"/>
+      <c r="K12" s="45"/>
+      <c r="L12" s="46"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E13" s="38">
+      <c r="E13" s="41">
         <v>44664</v>
       </c>
-      <c r="F13" s="39"/>
+      <c r="F13" s="42"/>
       <c r="G13" s="18">
         <v>3</v>
       </c>
-      <c r="H13" s="15" t="str">
+      <c r="H13" s="33" t="str">
         <f>_xlfn.XLOOKUP(Bracket!G13,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
         <v>Cosmic Brownie</v>
       </c>
-      <c r="I13" s="28"/>
-      <c r="K13" s="42"/>
-      <c r="L13" s="43"/>
+      <c r="I13" s="37">
+        <v>0</v>
+      </c>
+      <c r="K13" s="45"/>
+      <c r="L13" s="46"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E14" s="40"/>
-      <c r="F14" s="41"/>
-      <c r="K14" s="42"/>
-      <c r="L14" s="43"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="44"/>
+      <c r="K14" s="45"/>
+      <c r="L14" s="46"/>
       <c r="M14" s="18"/>
       <c r="N14" s="15" t="str">
         <f>_xlfn.XLOOKUP(Bracket!M14,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
@@ -1406,18 +1412,18 @@
       <c r="F15" s="35">
         <v>2</v>
       </c>
-      <c r="K15" s="42"/>
-      <c r="L15" s="43"/>
-      <c r="N15" s="38">
+      <c r="K15" s="45"/>
+      <c r="L15" s="46"/>
+      <c r="N15" s="41">
         <v>44685</v>
       </c>
-      <c r="O15" s="39"/>
+      <c r="O15" s="42"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="K16" s="42"/>
-      <c r="L16" s="43"/>
-      <c r="N16" s="42"/>
-      <c r="O16" s="43"/>
+      <c r="K16" s="45"/>
+      <c r="L16" s="46"/>
+      <c r="N16" s="45"/>
+      <c r="O16" s="46"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D17" s="16">
@@ -1430,16 +1436,16 @@
       <c r="F17" s="34">
         <v>5</v>
       </c>
-      <c r="K17" s="42"/>
-      <c r="L17" s="43"/>
-      <c r="N17" s="42"/>
-      <c r="O17" s="43"/>
+      <c r="K17" s="45"/>
+      <c r="L17" s="46"/>
+      <c r="N17" s="45"/>
+      <c r="O17" s="46"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E18" s="38">
+      <c r="E18" s="41">
         <v>44665</v>
       </c>
-      <c r="F18" s="39"/>
+      <c r="F18" s="42"/>
       <c r="G18" s="18">
         <v>5</v>
       </c>
@@ -1450,22 +1456,22 @@
       <c r="I18" s="34">
         <v>3</v>
       </c>
-      <c r="K18" s="42"/>
-      <c r="L18" s="43"/>
-      <c r="N18" s="42"/>
-      <c r="O18" s="43"/>
+      <c r="K18" s="45"/>
+      <c r="L18" s="46"/>
+      <c r="N18" s="45"/>
+      <c r="O18" s="46"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E19" s="40"/>
-      <c r="F19" s="41"/>
-      <c r="H19" s="38">
+      <c r="E19" s="43"/>
+      <c r="F19" s="44"/>
+      <c r="H19" s="41">
         <v>44677</v>
       </c>
-      <c r="I19" s="39"/>
-      <c r="K19" s="40"/>
-      <c r="L19" s="41"/>
-      <c r="N19" s="42"/>
-      <c r="O19" s="43"/>
+      <c r="I19" s="42"/>
+      <c r="K19" s="43"/>
+      <c r="L19" s="44"/>
+      <c r="N19" s="45"/>
+      <c r="O19" s="46"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D20" s="16">
@@ -1478,8 +1484,8 @@
       <c r="F20" s="35">
         <v>0</v>
       </c>
-      <c r="H20" s="42"/>
-      <c r="I20" s="43"/>
+      <c r="H20" s="45"/>
+      <c r="I20" s="46"/>
       <c r="J20" s="18">
         <v>5</v>
       </c>
@@ -1488,14 +1494,14 @@
         <v>Star Crunch</v>
       </c>
       <c r="L20" s="28"/>
-      <c r="N20" s="42"/>
-      <c r="O20" s="43"/>
+      <c r="N20" s="45"/>
+      <c r="O20" s="46"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="H21" s="42"/>
-      <c r="I21" s="43"/>
-      <c r="N21" s="42"/>
-      <c r="O21" s="43"/>
+      <c r="H21" s="45"/>
+      <c r="I21" s="46"/>
+      <c r="N21" s="45"/>
+      <c r="O21" s="46"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D22" s="16">
@@ -1508,16 +1514,16 @@
       <c r="F22" s="34">
         <v>4</v>
       </c>
-      <c r="H22" s="40"/>
-      <c r="I22" s="41"/>
-      <c r="N22" s="42"/>
-      <c r="O22" s="43"/>
+      <c r="H22" s="43"/>
+      <c r="I22" s="44"/>
+      <c r="N22" s="45"/>
+      <c r="O22" s="46"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E23" s="38">
+      <c r="E23" s="41">
         <v>44669</v>
       </c>
-      <c r="F23" s="39"/>
+      <c r="F23" s="42"/>
       <c r="G23" s="18">
         <v>7</v>
       </c>
@@ -1525,11 +1531,11 @@
         <f>_xlfn.XLOOKUP(Bracket!G23,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
         <v>Fudge Rounds</v>
       </c>
-      <c r="I23" s="32">
+      <c r="I23" s="37">
         <v>2</v>
       </c>
-      <c r="N23" s="42"/>
-      <c r="O23" s="43"/>
+      <c r="N23" s="45"/>
+      <c r="O23" s="46"/>
       <c r="P23" s="18"/>
       <c r="Q23" s="15" t="str">
         <f>_xlfn.XLOOKUP(Bracket!P23,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
@@ -1539,10 +1545,10 @@
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
-      <c r="E24" s="40"/>
-      <c r="F24" s="41"/>
-      <c r="N24" s="42"/>
-      <c r="O24" s="43"/>
+      <c r="E24" s="43"/>
+      <c r="F24" s="44"/>
+      <c r="N24" s="45"/>
+      <c r="O24" s="46"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B25" s="9"/>
@@ -1557,14 +1563,14 @@
       <c r="F25" s="35">
         <v>2</v>
       </c>
-      <c r="N25" s="42"/>
-      <c r="O25" s="43"/>
+      <c r="N25" s="45"/>
+      <c r="O25" s="46"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
-      <c r="N26" s="42"/>
-      <c r="O26" s="43"/>
+      <c r="N26" s="45"/>
+      <c r="O26" s="46"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B27" s="9"/>
@@ -1579,24 +1585,26 @@
       <c r="F27" s="32">
         <v>2</v>
       </c>
-      <c r="N27" s="42"/>
-      <c r="O27" s="43"/>
+      <c r="N27" s="45"/>
+      <c r="O27" s="46"/>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E28" s="38">
+      <c r="E28" s="41">
         <v>44671</v>
       </c>
-      <c r="F28" s="39"/>
+      <c r="F28" s="42"/>
       <c r="G28" s="18">
         <v>18</v>
       </c>
-      <c r="H28" s="15" t="str">
+      <c r="H28" s="33" t="str">
         <f>_xlfn.XLOOKUP(Bracket!G28,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
         <v>Chocolate Chip Cream Pies</v>
       </c>
-      <c r="I28" s="27"/>
-      <c r="N28" s="42"/>
-      <c r="O28" s="43"/>
+      <c r="I28" s="37">
+        <v>0</v>
+      </c>
+      <c r="N28" s="45"/>
+      <c r="O28" s="46"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="16">
@@ -1609,20 +1617,20 @@
       <c r="C29" s="32">
         <v>3</v>
       </c>
-      <c r="E29" s="40"/>
-      <c r="F29" s="41"/>
-      <c r="H29" s="38">
+      <c r="E29" s="43"/>
+      <c r="F29" s="44"/>
+      <c r="H29" s="41">
         <v>44679</v>
       </c>
-      <c r="I29" s="39"/>
-      <c r="N29" s="42"/>
-      <c r="O29" s="43"/>
+      <c r="I29" s="42"/>
+      <c r="N29" s="45"/>
+      <c r="O29" s="46"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B30" s="38">
+      <c r="B30" s="41">
         <v>44670</v>
       </c>
-      <c r="C30" s="39"/>
+      <c r="C30" s="42"/>
       <c r="D30" s="18">
         <v>18</v>
       </c>
@@ -1633,28 +1641,30 @@
       <c r="F30" s="31">
         <v>3</v>
       </c>
-      <c r="H30" s="42"/>
-      <c r="I30" s="43"/>
-      <c r="J30" s="18"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="46"/>
+      <c r="J30" s="18">
+        <v>6</v>
+      </c>
       <c r="K30" s="15" t="str">
         <f>_xlfn.XLOOKUP(Bracket!J30,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
-        <v>TBD</v>
+        <v>Oatmeal Cream Pies</v>
       </c>
       <c r="L30" s="27"/>
-      <c r="N30" s="42"/>
-      <c r="O30" s="43"/>
+      <c r="N30" s="45"/>
+      <c r="O30" s="46"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B31" s="40"/>
-      <c r="C31" s="41"/>
-      <c r="H31" s="42"/>
-      <c r="I31" s="43"/>
-      <c r="K31" s="38">
+      <c r="B31" s="43"/>
+      <c r="C31" s="44"/>
+      <c r="H31" s="45"/>
+      <c r="I31" s="46"/>
+      <c r="K31" s="41">
         <v>44684</v>
       </c>
-      <c r="L31" s="39"/>
-      <c r="N31" s="42"/>
-      <c r="O31" s="43"/>
+      <c r="L31" s="42"/>
+      <c r="N31" s="45"/>
+      <c r="O31" s="46"/>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="16">
@@ -1677,36 +1687,38 @@
       <c r="F32" s="34">
         <v>4</v>
       </c>
-      <c r="H32" s="40"/>
-      <c r="I32" s="41"/>
-      <c r="K32" s="42"/>
-      <c r="L32" s="43"/>
-      <c r="N32" s="42"/>
-      <c r="O32" s="43"/>
+      <c r="H32" s="43"/>
+      <c r="I32" s="44"/>
+      <c r="K32" s="45"/>
+      <c r="L32" s="46"/>
+      <c r="N32" s="45"/>
+      <c r="O32" s="46"/>
     </row>
     <row r="33" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="E33" s="38">
+      <c r="E33" s="41">
         <v>44672</v>
       </c>
-      <c r="F33" s="39"/>
+      <c r="F33" s="42"/>
       <c r="G33" s="18">
         <v>6</v>
       </c>
-      <c r="H33" s="15" t="str">
+      <c r="H33" s="30" t="str">
         <f>_xlfn.XLOOKUP(Bracket!G33,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
         <v>Oatmeal Cream Pies</v>
       </c>
-      <c r="I33" s="28"/>
-      <c r="K33" s="42"/>
-      <c r="L33" s="43"/>
-      <c r="N33" s="40"/>
-      <c r="O33" s="41"/>
+      <c r="I33" s="30">
+        <v>4</v>
+      </c>
+      <c r="K33" s="45"/>
+      <c r="L33" s="46"/>
+      <c r="N33" s="43"/>
+      <c r="O33" s="44"/>
     </row>
     <row r="34" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="E34" s="40"/>
-      <c r="F34" s="41"/>
-      <c r="K34" s="42"/>
-      <c r="L34" s="43"/>
+      <c r="E34" s="43"/>
+      <c r="F34" s="44"/>
+      <c r="K34" s="45"/>
+      <c r="L34" s="46"/>
       <c r="M34" s="18"/>
       <c r="N34" s="15" t="str">
         <f>_xlfn.XLOOKUP(Bracket!M34,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
@@ -1725,12 +1737,12 @@
       <c r="F35" s="35">
         <v>1</v>
       </c>
-      <c r="K35" s="42"/>
-      <c r="L35" s="43"/>
+      <c r="K35" s="45"/>
+      <c r="L35" s="46"/>
     </row>
     <row r="36" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="K36" s="42"/>
-      <c r="L36" s="43"/>
+      <c r="K36" s="45"/>
+      <c r="L36" s="46"/>
     </row>
     <row r="37" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D37" s="16">
@@ -1743,14 +1755,14 @@
       <c r="F37" s="34">
         <v>5</v>
       </c>
-      <c r="K37" s="42"/>
-      <c r="L37" s="43"/>
+      <c r="K37" s="45"/>
+      <c r="L37" s="46"/>
     </row>
     <row r="38" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="E38" s="38">
+      <c r="E38" s="41">
         <v>44673</v>
       </c>
-      <c r="F38" s="39"/>
+      <c r="F38" s="42"/>
       <c r="G38" s="18">
         <v>4</v>
       </c>
@@ -1759,18 +1771,18 @@
         <v>Nutty Buddy</v>
       </c>
       <c r="I38" s="27"/>
-      <c r="K38" s="42"/>
-      <c r="L38" s="43"/>
+      <c r="K38" s="45"/>
+      <c r="L38" s="46"/>
     </row>
     <row r="39" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="E39" s="40"/>
-      <c r="F39" s="41"/>
-      <c r="H39" s="38">
+      <c r="E39" s="43"/>
+      <c r="F39" s="44"/>
+      <c r="H39" s="41">
         <v>44680</v>
       </c>
-      <c r="I39" s="39"/>
-      <c r="K39" s="40"/>
-      <c r="L39" s="41"/>
+      <c r="I39" s="42"/>
+      <c r="K39" s="43"/>
+      <c r="L39" s="44"/>
     </row>
     <row r="40" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D40" s="16">
@@ -1783,8 +1795,8 @@
       <c r="F40" s="35">
         <v>1</v>
       </c>
-      <c r="H40" s="42"/>
-      <c r="I40" s="43"/>
+      <c r="H40" s="45"/>
+      <c r="I40" s="46"/>
       <c r="J40" s="18"/>
       <c r="K40" s="15" t="str">
         <f>_xlfn.XLOOKUP(Bracket!J40,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
@@ -1793,8 +1805,8 @@
       <c r="L40" s="28"/>
     </row>
     <row r="41" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="H41" s="42"/>
-      <c r="I41" s="43"/>
+      <c r="H41" s="45"/>
+      <c r="I41" s="46"/>
     </row>
     <row r="42" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D42" s="16">
@@ -1807,14 +1819,14 @@
       <c r="F42" s="37">
         <v>1</v>
       </c>
-      <c r="H42" s="40"/>
-      <c r="I42" s="41"/>
+      <c r="H42" s="43"/>
+      <c r="I42" s="44"/>
     </row>
     <row r="43" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="E43" s="38">
+      <c r="E43" s="41">
         <v>44676</v>
       </c>
-      <c r="F43" s="39"/>
+      <c r="F43" s="42"/>
       <c r="G43" s="18">
         <v>9</v>
       </c>
@@ -1827,8 +1839,8 @@
     <row r="44" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B44" s="9"/>
       <c r="C44" s="9"/>
-      <c r="E44" s="40"/>
-      <c r="F44" s="41"/>
+      <c r="E44" s="43"/>
+      <c r="F44" s="44"/>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45" s="9"/>
@@ -1854,6 +1866,11 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="E43:F44"/>
+    <mergeCell ref="H29:I32"/>
+    <mergeCell ref="H39:I42"/>
+    <mergeCell ref="B30:C31"/>
+    <mergeCell ref="E23:F24"/>
     <mergeCell ref="B2:Q2"/>
     <mergeCell ref="B10:C11"/>
     <mergeCell ref="E8:F9"/>
@@ -1867,11 +1884,6 @@
     <mergeCell ref="E33:F34"/>
     <mergeCell ref="K31:L39"/>
     <mergeCell ref="E38:F39"/>
-    <mergeCell ref="E43:F44"/>
-    <mergeCell ref="H29:I32"/>
-    <mergeCell ref="H39:I42"/>
-    <mergeCell ref="B30:C31"/>
-    <mergeCell ref="E23:F24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
4/29 - Nutty Buddy Wins!
</commit_message>
<xml_diff>
--- a/LilDebBracket.xlsx
+++ b/LilDebBracket.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdd45780\Documents\GitHub\lildeb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDA87C47-B3DF-480C-85B5-8B478F21A855}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E5F7E92-F189-4DFC-B03F-793BA7D32A3A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35730" yWindow="14730" windowWidth="43200" windowHeight="23535" xr2:uid="{10960CD5-A4F3-447E-9C42-3300723A7601}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{10960CD5-A4F3-447E-9C42-3300723A7601}"/>
   </bookViews>
   <sheets>
     <sheet name="Bracket" sheetId="3" r:id="rId1"/>
@@ -633,15 +633,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="16" fontId="4" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -659,6 +650,15 @@
     </xf>
     <xf numFmtId="16" fontId="4" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1178,8 +1178,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0E5BB06-8011-4308-BEC9-9A7436B98035}">
   <dimension ref="A1:Q47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="K45" sqref="K45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1201,24 +1201,24 @@
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:17" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
-      <c r="M2" s="39"/>
-      <c r="N2" s="39"/>
-      <c r="O2" s="39"/>
-      <c r="P2" s="39"/>
-      <c r="Q2" s="40"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="45"/>
+      <c r="L2" s="45"/>
+      <c r="M2" s="45"/>
+      <c r="N2" s="45"/>
+      <c r="O2" s="45"/>
+      <c r="P2" s="45"/>
+      <c r="Q2" s="46"/>
     </row>
     <row r="3" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B3" s="11"/>
@@ -1276,10 +1276,10 @@
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E8" s="41">
+      <c r="E8" s="38">
         <v>44663</v>
       </c>
-      <c r="F8" s="42"/>
+      <c r="F8" s="39"/>
       <c r="G8" s="18">
         <v>17</v>
       </c>
@@ -1302,18 +1302,18 @@
       <c r="C9" s="32">
         <v>2</v>
       </c>
-      <c r="E9" s="43"/>
-      <c r="F9" s="44"/>
-      <c r="H9" s="41">
+      <c r="E9" s="40"/>
+      <c r="F9" s="41"/>
+      <c r="H9" s="38">
         <v>44679</v>
       </c>
-      <c r="I9" s="42"/>
+      <c r="I9" s="39"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B10" s="41">
+      <c r="B10" s="38">
         <v>44662</v>
       </c>
-      <c r="C10" s="42"/>
+      <c r="C10" s="39"/>
       <c r="D10" s="18">
         <v>17</v>
       </c>
@@ -1324,8 +1324,8 @@
       <c r="F10" s="31">
         <v>4</v>
       </c>
-      <c r="H10" s="45"/>
-      <c r="I10" s="46"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="43"/>
       <c r="J10" s="18">
         <v>17</v>
       </c>
@@ -1336,14 +1336,14 @@
       <c r="L10" s="27"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B11" s="43"/>
-      <c r="C11" s="44"/>
-      <c r="H11" s="45"/>
-      <c r="I11" s="46"/>
-      <c r="K11" s="41">
+      <c r="B11" s="40"/>
+      <c r="C11" s="41"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="43"/>
+      <c r="K11" s="38">
         <v>44683</v>
       </c>
-      <c r="L11" s="42"/>
+      <c r="L11" s="39"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="16">
@@ -1366,16 +1366,16 @@
       <c r="F12" s="34">
         <v>3</v>
       </c>
-      <c r="H12" s="43"/>
-      <c r="I12" s="44"/>
-      <c r="K12" s="45"/>
-      <c r="L12" s="46"/>
+      <c r="H12" s="40"/>
+      <c r="I12" s="41"/>
+      <c r="K12" s="42"/>
+      <c r="L12" s="43"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E13" s="41">
+      <c r="E13" s="38">
         <v>44664</v>
       </c>
-      <c r="F13" s="42"/>
+      <c r="F13" s="39"/>
       <c r="G13" s="18">
         <v>3</v>
       </c>
@@ -1386,14 +1386,14 @@
       <c r="I13" s="37">
         <v>0</v>
       </c>
-      <c r="K13" s="45"/>
-      <c r="L13" s="46"/>
+      <c r="K13" s="42"/>
+      <c r="L13" s="43"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E14" s="43"/>
-      <c r="F14" s="44"/>
-      <c r="K14" s="45"/>
-      <c r="L14" s="46"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="41"/>
+      <c r="K14" s="42"/>
+      <c r="L14" s="43"/>
       <c r="M14" s="18"/>
       <c r="N14" s="15" t="str">
         <f>_xlfn.XLOOKUP(Bracket!M14,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
@@ -1412,18 +1412,18 @@
       <c r="F15" s="35">
         <v>2</v>
       </c>
-      <c r="K15" s="45"/>
-      <c r="L15" s="46"/>
-      <c r="N15" s="41">
+      <c r="K15" s="42"/>
+      <c r="L15" s="43"/>
+      <c r="N15" s="38">
         <v>44685</v>
       </c>
-      <c r="O15" s="42"/>
+      <c r="O15" s="39"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="K16" s="45"/>
-      <c r="L16" s="46"/>
-      <c r="N16" s="45"/>
-      <c r="O16" s="46"/>
+      <c r="K16" s="42"/>
+      <c r="L16" s="43"/>
+      <c r="N16" s="42"/>
+      <c r="O16" s="43"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D17" s="16">
@@ -1436,16 +1436,16 @@
       <c r="F17" s="34">
         <v>5</v>
       </c>
-      <c r="K17" s="45"/>
-      <c r="L17" s="46"/>
-      <c r="N17" s="45"/>
-      <c r="O17" s="46"/>
+      <c r="K17" s="42"/>
+      <c r="L17" s="43"/>
+      <c r="N17" s="42"/>
+      <c r="O17" s="43"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E18" s="41">
+      <c r="E18" s="38">
         <v>44665</v>
       </c>
-      <c r="F18" s="42"/>
+      <c r="F18" s="39"/>
       <c r="G18" s="18">
         <v>5</v>
       </c>
@@ -1456,22 +1456,22 @@
       <c r="I18" s="34">
         <v>3</v>
       </c>
-      <c r="K18" s="45"/>
-      <c r="L18" s="46"/>
-      <c r="N18" s="45"/>
-      <c r="O18" s="46"/>
+      <c r="K18" s="42"/>
+      <c r="L18" s="43"/>
+      <c r="N18" s="42"/>
+      <c r="O18" s="43"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E19" s="43"/>
-      <c r="F19" s="44"/>
-      <c r="H19" s="41">
+      <c r="E19" s="40"/>
+      <c r="F19" s="41"/>
+      <c r="H19" s="38">
         <v>44677</v>
       </c>
-      <c r="I19" s="42"/>
-      <c r="K19" s="43"/>
-      <c r="L19" s="44"/>
-      <c r="N19" s="45"/>
-      <c r="O19" s="46"/>
+      <c r="I19" s="39"/>
+      <c r="K19" s="40"/>
+      <c r="L19" s="41"/>
+      <c r="N19" s="42"/>
+      <c r="O19" s="43"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D20" s="16">
@@ -1484,8 +1484,8 @@
       <c r="F20" s="35">
         <v>0</v>
       </c>
-      <c r="H20" s="45"/>
-      <c r="I20" s="46"/>
+      <c r="H20" s="42"/>
+      <c r="I20" s="43"/>
       <c r="J20" s="18">
         <v>5</v>
       </c>
@@ -1494,14 +1494,14 @@
         <v>Star Crunch</v>
       </c>
       <c r="L20" s="28"/>
-      <c r="N20" s="45"/>
-      <c r="O20" s="46"/>
+      <c r="N20" s="42"/>
+      <c r="O20" s="43"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="H21" s="45"/>
-      <c r="I21" s="46"/>
-      <c r="N21" s="45"/>
-      <c r="O21" s="46"/>
+      <c r="H21" s="42"/>
+      <c r="I21" s="43"/>
+      <c r="N21" s="42"/>
+      <c r="O21" s="43"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D22" s="16">
@@ -1514,16 +1514,16 @@
       <c r="F22" s="34">
         <v>4</v>
       </c>
-      <c r="H22" s="43"/>
-      <c r="I22" s="44"/>
-      <c r="N22" s="45"/>
-      <c r="O22" s="46"/>
+      <c r="H22" s="40"/>
+      <c r="I22" s="41"/>
+      <c r="N22" s="42"/>
+      <c r="O22" s="43"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E23" s="41">
+      <c r="E23" s="38">
         <v>44669</v>
       </c>
-      <c r="F23" s="42"/>
+      <c r="F23" s="39"/>
       <c r="G23" s="18">
         <v>7</v>
       </c>
@@ -1534,8 +1534,8 @@
       <c r="I23" s="37">
         <v>2</v>
       </c>
-      <c r="N23" s="45"/>
-      <c r="O23" s="46"/>
+      <c r="N23" s="42"/>
+      <c r="O23" s="43"/>
       <c r="P23" s="18"/>
       <c r="Q23" s="15" t="str">
         <f>_xlfn.XLOOKUP(Bracket!P23,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
@@ -1545,10 +1545,10 @@
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
-      <c r="E24" s="43"/>
-      <c r="F24" s="44"/>
-      <c r="N24" s="45"/>
-      <c r="O24" s="46"/>
+      <c r="E24" s="40"/>
+      <c r="F24" s="41"/>
+      <c r="N24" s="42"/>
+      <c r="O24" s="43"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B25" s="9"/>
@@ -1563,14 +1563,14 @@
       <c r="F25" s="35">
         <v>2</v>
       </c>
-      <c r="N25" s="45"/>
-      <c r="O25" s="46"/>
+      <c r="N25" s="42"/>
+      <c r="O25" s="43"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
-      <c r="N26" s="45"/>
-      <c r="O26" s="46"/>
+      <c r="N26" s="42"/>
+      <c r="O26" s="43"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B27" s="9"/>
@@ -1585,14 +1585,14 @@
       <c r="F27" s="32">
         <v>2</v>
       </c>
-      <c r="N27" s="45"/>
-      <c r="O27" s="46"/>
+      <c r="N27" s="42"/>
+      <c r="O27" s="43"/>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E28" s="41">
+      <c r="E28" s="38">
         <v>44671</v>
       </c>
-      <c r="F28" s="42"/>
+      <c r="F28" s="39"/>
       <c r="G28" s="18">
         <v>18</v>
       </c>
@@ -1603,8 +1603,8 @@
       <c r="I28" s="37">
         <v>0</v>
       </c>
-      <c r="N28" s="45"/>
-      <c r="O28" s="46"/>
+      <c r="N28" s="42"/>
+      <c r="O28" s="43"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="16">
@@ -1617,20 +1617,20 @@
       <c r="C29" s="32">
         <v>3</v>
       </c>
-      <c r="E29" s="43"/>
-      <c r="F29" s="44"/>
-      <c r="H29" s="41">
+      <c r="E29" s="40"/>
+      <c r="F29" s="41"/>
+      <c r="H29" s="38">
         <v>44679</v>
       </c>
-      <c r="I29" s="42"/>
-      <c r="N29" s="45"/>
-      <c r="O29" s="46"/>
+      <c r="I29" s="39"/>
+      <c r="N29" s="42"/>
+      <c r="O29" s="43"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B30" s="41">
+      <c r="B30" s="38">
         <v>44670</v>
       </c>
-      <c r="C30" s="42"/>
+      <c r="C30" s="39"/>
       <c r="D30" s="18">
         <v>18</v>
       </c>
@@ -1641,8 +1641,8 @@
       <c r="F30" s="31">
         <v>3</v>
       </c>
-      <c r="H30" s="45"/>
-      <c r="I30" s="46"/>
+      <c r="H30" s="42"/>
+      <c r="I30" s="43"/>
       <c r="J30" s="18">
         <v>6</v>
       </c>
@@ -1651,20 +1651,20 @@
         <v>Oatmeal Cream Pies</v>
       </c>
       <c r="L30" s="27"/>
-      <c r="N30" s="45"/>
-      <c r="O30" s="46"/>
+      <c r="N30" s="42"/>
+      <c r="O30" s="43"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B31" s="43"/>
-      <c r="C31" s="44"/>
-      <c r="H31" s="45"/>
-      <c r="I31" s="46"/>
-      <c r="K31" s="41">
+      <c r="B31" s="40"/>
+      <c r="C31" s="41"/>
+      <c r="H31" s="42"/>
+      <c r="I31" s="43"/>
+      <c r="K31" s="38">
         <v>44684</v>
       </c>
-      <c r="L31" s="42"/>
-      <c r="N31" s="45"/>
-      <c r="O31" s="46"/>
+      <c r="L31" s="39"/>
+      <c r="N31" s="42"/>
+      <c r="O31" s="43"/>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="16">
@@ -1687,18 +1687,18 @@
       <c r="F32" s="34">
         <v>4</v>
       </c>
-      <c r="H32" s="43"/>
-      <c r="I32" s="44"/>
-      <c r="K32" s="45"/>
-      <c r="L32" s="46"/>
-      <c r="N32" s="45"/>
-      <c r="O32" s="46"/>
+      <c r="H32" s="40"/>
+      <c r="I32" s="41"/>
+      <c r="K32" s="42"/>
+      <c r="L32" s="43"/>
+      <c r="N32" s="42"/>
+      <c r="O32" s="43"/>
     </row>
     <row r="33" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="E33" s="41">
+      <c r="E33" s="38">
         <v>44672</v>
       </c>
-      <c r="F33" s="42"/>
+      <c r="F33" s="39"/>
       <c r="G33" s="18">
         <v>6</v>
       </c>
@@ -1709,16 +1709,16 @@
       <c r="I33" s="30">
         <v>4</v>
       </c>
-      <c r="K33" s="45"/>
-      <c r="L33" s="46"/>
-      <c r="N33" s="43"/>
-      <c r="O33" s="44"/>
+      <c r="K33" s="42"/>
+      <c r="L33" s="43"/>
+      <c r="N33" s="40"/>
+      <c r="O33" s="41"/>
     </row>
     <row r="34" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="E34" s="43"/>
-      <c r="F34" s="44"/>
-      <c r="K34" s="45"/>
-      <c r="L34" s="46"/>
+      <c r="E34" s="40"/>
+      <c r="F34" s="41"/>
+      <c r="K34" s="42"/>
+      <c r="L34" s="43"/>
       <c r="M34" s="18"/>
       <c r="N34" s="15" t="str">
         <f>_xlfn.XLOOKUP(Bracket!M34,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
@@ -1737,12 +1737,12 @@
       <c r="F35" s="35">
         <v>1</v>
       </c>
-      <c r="K35" s="45"/>
-      <c r="L35" s="46"/>
+      <c r="K35" s="42"/>
+      <c r="L35" s="43"/>
     </row>
     <row r="36" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="K36" s="45"/>
-      <c r="L36" s="46"/>
+      <c r="K36" s="42"/>
+      <c r="L36" s="43"/>
     </row>
     <row r="37" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D37" s="16">
@@ -1755,34 +1755,36 @@
       <c r="F37" s="34">
         <v>5</v>
       </c>
-      <c r="K37" s="45"/>
-      <c r="L37" s="46"/>
+      <c r="K37" s="42"/>
+      <c r="L37" s="43"/>
     </row>
     <row r="38" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="E38" s="41">
+      <c r="E38" s="38">
         <v>44673</v>
       </c>
-      <c r="F38" s="42"/>
+      <c r="F38" s="39"/>
       <c r="G38" s="18">
         <v>4</v>
       </c>
-      <c r="H38" s="15" t="str">
+      <c r="H38" s="30" t="str">
         <f>_xlfn.XLOOKUP(Bracket!G38,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
         <v>Nutty Buddy</v>
       </c>
-      <c r="I38" s="27"/>
-      <c r="K38" s="45"/>
-      <c r="L38" s="46"/>
+      <c r="I38" s="34">
+        <v>3</v>
+      </c>
+      <c r="K38" s="42"/>
+      <c r="L38" s="43"/>
     </row>
     <row r="39" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="E39" s="43"/>
-      <c r="F39" s="44"/>
-      <c r="H39" s="41">
+      <c r="E39" s="40"/>
+      <c r="F39" s="41"/>
+      <c r="H39" s="38">
         <v>44680</v>
       </c>
-      <c r="I39" s="42"/>
-      <c r="K39" s="43"/>
-      <c r="L39" s="44"/>
+      <c r="I39" s="39"/>
+      <c r="K39" s="40"/>
+      <c r="L39" s="41"/>
     </row>
     <row r="40" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D40" s="16">
@@ -1795,18 +1797,20 @@
       <c r="F40" s="35">
         <v>1</v>
       </c>
-      <c r="H40" s="45"/>
-      <c r="I40" s="46"/>
-      <c r="J40" s="18"/>
+      <c r="H40" s="42"/>
+      <c r="I40" s="43"/>
+      <c r="J40" s="18">
+        <v>4</v>
+      </c>
       <c r="K40" s="15" t="str">
         <f>_xlfn.XLOOKUP(Bracket!J40,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
-        <v>TBD</v>
+        <v>Nutty Buddy</v>
       </c>
       <c r="L40" s="28"/>
     </row>
     <row r="41" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="H41" s="45"/>
-      <c r="I41" s="46"/>
+      <c r="H41" s="42"/>
+      <c r="I41" s="43"/>
     </row>
     <row r="42" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D42" s="16">
@@ -1819,28 +1823,30 @@
       <c r="F42" s="37">
         <v>1</v>
       </c>
-      <c r="H42" s="43"/>
-      <c r="I42" s="44"/>
+      <c r="H42" s="40"/>
+      <c r="I42" s="41"/>
     </row>
     <row r="43" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="E43" s="41">
+      <c r="E43" s="38">
         <v>44676</v>
       </c>
-      <c r="F43" s="42"/>
+      <c r="F43" s="39"/>
       <c r="G43" s="18">
         <v>9</v>
       </c>
-      <c r="H43" s="15" t="str">
+      <c r="H43" s="33" t="str">
         <f>_xlfn.XLOOKUP(Bracket!G43,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
         <v>Peanut Butter Cream Pies</v>
       </c>
-      <c r="I43" s="28"/>
+      <c r="I43" s="37">
+        <v>1</v>
+      </c>
     </row>
     <row r="44" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B44" s="9"/>
       <c r="C44" s="9"/>
-      <c r="E44" s="43"/>
-      <c r="F44" s="44"/>
+      <c r="E44" s="40"/>
+      <c r="F44" s="41"/>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45" s="9"/>
@@ -1866,11 +1872,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="E43:F44"/>
-    <mergeCell ref="H29:I32"/>
-    <mergeCell ref="H39:I42"/>
-    <mergeCell ref="B30:C31"/>
-    <mergeCell ref="E23:F24"/>
     <mergeCell ref="B2:Q2"/>
     <mergeCell ref="B10:C11"/>
     <mergeCell ref="E8:F9"/>
@@ -1884,6 +1885,11 @@
     <mergeCell ref="E33:F34"/>
     <mergeCell ref="K31:L39"/>
     <mergeCell ref="E38:F39"/>
+    <mergeCell ref="E43:F44"/>
+    <mergeCell ref="H29:I32"/>
+    <mergeCell ref="H39:I42"/>
+    <mergeCell ref="B30:C31"/>
+    <mergeCell ref="E23:F24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Peanut Butter Crunch continues the cinderella run
</commit_message>
<xml_diff>
--- a/LilDebBracket.xlsx
+++ b/LilDebBracket.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdd45780\Documents\GitHub\lildeb\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kwiktrip-my.sharepoint.com/personal/am10014003_kwiktrip_com/Documents/Development/lildeb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E5F7E92-F189-4DFC-B03F-793BA7D32A3A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{6E5F7E92-F189-4DFC-B03F-793BA7D32A3A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{5A6CE12B-4652-44AB-BB0E-1E953A01B951}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{10960CD5-A4F3-447E-9C42-3300723A7601}"/>
   </bookViews>
@@ -633,6 +633,15 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="16" fontId="4" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -650,15 +659,6 @@
     </xf>
     <xf numFmtId="16" fontId="4" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1178,9 +1178,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0E5BB06-8011-4308-BEC9-9A7436B98035}">
   <dimension ref="A1:Q47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K45" sqref="K45"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1194,31 +1192,31 @@
     <col min="9" max="9" width="3.7109375" customWidth="1"/>
     <col min="11" max="11" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="3.7109375" customWidth="1"/>
-    <col min="14" max="14" width="14" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="3.7109375" customWidth="1"/>
     <col min="17" max="17" width="7.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:17" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="45"/>
-      <c r="M2" s="45"/>
-      <c r="N2" s="45"/>
-      <c r="O2" s="45"/>
-      <c r="P2" s="45"/>
-      <c r="Q2" s="46"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
+      <c r="N2" s="39"/>
+      <c r="O2" s="39"/>
+      <c r="P2" s="39"/>
+      <c r="Q2" s="40"/>
     </row>
     <row r="3" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B3" s="11"/>
@@ -1276,10 +1274,10 @@
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E8" s="38">
+      <c r="E8" s="41">
         <v>44663</v>
       </c>
-      <c r="F8" s="39"/>
+      <c r="F8" s="42"/>
       <c r="G8" s="18">
         <v>17</v>
       </c>
@@ -1302,18 +1300,18 @@
       <c r="C9" s="32">
         <v>2</v>
       </c>
-      <c r="E9" s="40"/>
-      <c r="F9" s="41"/>
-      <c r="H9" s="38">
+      <c r="E9" s="43"/>
+      <c r="F9" s="44"/>
+      <c r="H9" s="41">
         <v>44679</v>
       </c>
-      <c r="I9" s="39"/>
+      <c r="I9" s="42"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B10" s="38">
+      <c r="B10" s="41">
         <v>44662</v>
       </c>
-      <c r="C10" s="39"/>
+      <c r="C10" s="42"/>
       <c r="D10" s="18">
         <v>17</v>
       </c>
@@ -1324,26 +1322,28 @@
       <c r="F10" s="31">
         <v>4</v>
       </c>
-      <c r="H10" s="42"/>
-      <c r="I10" s="43"/>
+      <c r="H10" s="45"/>
+      <c r="I10" s="46"/>
       <c r="J10" s="18">
         <v>17</v>
       </c>
-      <c r="K10" s="15" t="str">
+      <c r="K10" s="30" t="str">
         <f>_xlfn.XLOOKUP(Bracket!J10,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
         <v>Peanut Butter Crunch</v>
       </c>
-      <c r="L10" s="27"/>
+      <c r="L10" s="34">
+        <v>4</v>
+      </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B11" s="40"/>
-      <c r="C11" s="41"/>
-      <c r="H11" s="42"/>
-      <c r="I11" s="43"/>
-      <c r="K11" s="38">
+      <c r="B11" s="43"/>
+      <c r="C11" s="44"/>
+      <c r="H11" s="45"/>
+      <c r="I11" s="46"/>
+      <c r="K11" s="41">
         <v>44683</v>
       </c>
-      <c r="L11" s="39"/>
+      <c r="L11" s="42"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="16">
@@ -1366,16 +1366,16 @@
       <c r="F12" s="34">
         <v>3</v>
       </c>
-      <c r="H12" s="40"/>
-      <c r="I12" s="41"/>
-      <c r="K12" s="42"/>
-      <c r="L12" s="43"/>
+      <c r="H12" s="43"/>
+      <c r="I12" s="44"/>
+      <c r="K12" s="45"/>
+      <c r="L12" s="46"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E13" s="38">
+      <c r="E13" s="41">
         <v>44664</v>
       </c>
-      <c r="F13" s="39"/>
+      <c r="F13" s="42"/>
       <c r="G13" s="18">
         <v>3</v>
       </c>
@@ -1386,18 +1386,20 @@
       <c r="I13" s="37">
         <v>0</v>
       </c>
-      <c r="K13" s="42"/>
-      <c r="L13" s="43"/>
+      <c r="K13" s="45"/>
+      <c r="L13" s="46"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E14" s="40"/>
-      <c r="F14" s="41"/>
-      <c r="K14" s="42"/>
-      <c r="L14" s="43"/>
-      <c r="M14" s="18"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="44"/>
+      <c r="K14" s="45"/>
+      <c r="L14" s="46"/>
+      <c r="M14" s="18">
+        <v>17</v>
+      </c>
       <c r="N14" s="15" t="str">
         <f>_xlfn.XLOOKUP(Bracket!M14,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
-        <v>TBD</v>
+        <v>Peanut Butter Crunch</v>
       </c>
       <c r="O14" s="27"/>
     </row>
@@ -1412,18 +1414,18 @@
       <c r="F15" s="35">
         <v>2</v>
       </c>
-      <c r="K15" s="42"/>
-      <c r="L15" s="43"/>
-      <c r="N15" s="38">
+      <c r="K15" s="45"/>
+      <c r="L15" s="46"/>
+      <c r="N15" s="41">
         <v>44685</v>
       </c>
-      <c r="O15" s="39"/>
+      <c r="O15" s="42"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="K16" s="42"/>
-      <c r="L16" s="43"/>
-      <c r="N16" s="42"/>
-      <c r="O16" s="43"/>
+      <c r="K16" s="45"/>
+      <c r="L16" s="46"/>
+      <c r="N16" s="45"/>
+      <c r="O16" s="46"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D17" s="16">
@@ -1436,16 +1438,16 @@
       <c r="F17" s="34">
         <v>5</v>
       </c>
-      <c r="K17" s="42"/>
-      <c r="L17" s="43"/>
-      <c r="N17" s="42"/>
-      <c r="O17" s="43"/>
+      <c r="K17" s="45"/>
+      <c r="L17" s="46"/>
+      <c r="N17" s="45"/>
+      <c r="O17" s="46"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E18" s="38">
+      <c r="E18" s="41">
         <v>44665</v>
       </c>
-      <c r="F18" s="39"/>
+      <c r="F18" s="42"/>
       <c r="G18" s="18">
         <v>5</v>
       </c>
@@ -1456,22 +1458,22 @@
       <c r="I18" s="34">
         <v>3</v>
       </c>
-      <c r="K18" s="42"/>
-      <c r="L18" s="43"/>
-      <c r="N18" s="42"/>
-      <c r="O18" s="43"/>
+      <c r="K18" s="45"/>
+      <c r="L18" s="46"/>
+      <c r="N18" s="45"/>
+      <c r="O18" s="46"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E19" s="40"/>
-      <c r="F19" s="41"/>
-      <c r="H19" s="38">
+      <c r="E19" s="43"/>
+      <c r="F19" s="44"/>
+      <c r="H19" s="41">
         <v>44677</v>
       </c>
-      <c r="I19" s="39"/>
-      <c r="K19" s="40"/>
-      <c r="L19" s="41"/>
-      <c r="N19" s="42"/>
-      <c r="O19" s="43"/>
+      <c r="I19" s="42"/>
+      <c r="K19" s="43"/>
+      <c r="L19" s="44"/>
+      <c r="N19" s="45"/>
+      <c r="O19" s="46"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D20" s="16">
@@ -1484,24 +1486,26 @@
       <c r="F20" s="35">
         <v>0</v>
       </c>
-      <c r="H20" s="42"/>
-      <c r="I20" s="43"/>
+      <c r="H20" s="45"/>
+      <c r="I20" s="46"/>
       <c r="J20" s="18">
         <v>5</v>
       </c>
-      <c r="K20" s="15" t="str">
+      <c r="K20" s="33" t="str">
         <f>_xlfn.XLOOKUP(Bracket!J20,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
         <v>Star Crunch</v>
       </c>
-      <c r="L20" s="28"/>
-      <c r="N20" s="42"/>
-      <c r="O20" s="43"/>
+      <c r="L20" s="35">
+        <v>2</v>
+      </c>
+      <c r="N20" s="45"/>
+      <c r="O20" s="46"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="H21" s="42"/>
-      <c r="I21" s="43"/>
-      <c r="N21" s="42"/>
-      <c r="O21" s="43"/>
+      <c r="H21" s="45"/>
+      <c r="I21" s="46"/>
+      <c r="N21" s="45"/>
+      <c r="O21" s="46"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D22" s="16">
@@ -1514,16 +1518,16 @@
       <c r="F22" s="34">
         <v>4</v>
       </c>
-      <c r="H22" s="40"/>
-      <c r="I22" s="41"/>
-      <c r="N22" s="42"/>
-      <c r="O22" s="43"/>
+      <c r="H22" s="43"/>
+      <c r="I22" s="44"/>
+      <c r="N22" s="45"/>
+      <c r="O22" s="46"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E23" s="38">
+      <c r="E23" s="41">
         <v>44669</v>
       </c>
-      <c r="F23" s="39"/>
+      <c r="F23" s="42"/>
       <c r="G23" s="18">
         <v>7</v>
       </c>
@@ -1534,8 +1538,8 @@
       <c r="I23" s="37">
         <v>2</v>
       </c>
-      <c r="N23" s="42"/>
-      <c r="O23" s="43"/>
+      <c r="N23" s="45"/>
+      <c r="O23" s="46"/>
       <c r="P23" s="18"/>
       <c r="Q23" s="15" t="str">
         <f>_xlfn.XLOOKUP(Bracket!P23,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
@@ -1545,10 +1549,10 @@
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
-      <c r="E24" s="40"/>
-      <c r="F24" s="41"/>
-      <c r="N24" s="42"/>
-      <c r="O24" s="43"/>
+      <c r="E24" s="43"/>
+      <c r="F24" s="44"/>
+      <c r="N24" s="45"/>
+      <c r="O24" s="46"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B25" s="9"/>
@@ -1563,14 +1567,14 @@
       <c r="F25" s="35">
         <v>2</v>
       </c>
-      <c r="N25" s="42"/>
-      <c r="O25" s="43"/>
+      <c r="N25" s="45"/>
+      <c r="O25" s="46"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
-      <c r="N26" s="42"/>
-      <c r="O26" s="43"/>
+      <c r="N26" s="45"/>
+      <c r="O26" s="46"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B27" s="9"/>
@@ -1585,14 +1589,14 @@
       <c r="F27" s="32">
         <v>2</v>
       </c>
-      <c r="N27" s="42"/>
-      <c r="O27" s="43"/>
+      <c r="N27" s="45"/>
+      <c r="O27" s="46"/>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E28" s="38">
+      <c r="E28" s="41">
         <v>44671</v>
       </c>
-      <c r="F28" s="39"/>
+      <c r="F28" s="42"/>
       <c r="G28" s="18">
         <v>18</v>
       </c>
@@ -1603,8 +1607,8 @@
       <c r="I28" s="37">
         <v>0</v>
       </c>
-      <c r="N28" s="42"/>
-      <c r="O28" s="43"/>
+      <c r="N28" s="45"/>
+      <c r="O28" s="46"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="16">
@@ -1617,20 +1621,20 @@
       <c r="C29" s="32">
         <v>3</v>
       </c>
-      <c r="E29" s="40"/>
-      <c r="F29" s="41"/>
-      <c r="H29" s="38">
+      <c r="E29" s="43"/>
+      <c r="F29" s="44"/>
+      <c r="H29" s="41">
         <v>44679</v>
       </c>
-      <c r="I29" s="39"/>
-      <c r="N29" s="42"/>
-      <c r="O29" s="43"/>
+      <c r="I29" s="42"/>
+      <c r="N29" s="45"/>
+      <c r="O29" s="46"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B30" s="38">
+      <c r="B30" s="41">
         <v>44670</v>
       </c>
-      <c r="C30" s="39"/>
+      <c r="C30" s="42"/>
       <c r="D30" s="18">
         <v>18</v>
       </c>
@@ -1641,8 +1645,8 @@
       <c r="F30" s="31">
         <v>3</v>
       </c>
-      <c r="H30" s="42"/>
-      <c r="I30" s="43"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="46"/>
       <c r="J30" s="18">
         <v>6</v>
       </c>
@@ -1651,20 +1655,20 @@
         <v>Oatmeal Cream Pies</v>
       </c>
       <c r="L30" s="27"/>
-      <c r="N30" s="42"/>
-      <c r="O30" s="43"/>
+      <c r="N30" s="45"/>
+      <c r="O30" s="46"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B31" s="40"/>
-      <c r="C31" s="41"/>
-      <c r="H31" s="42"/>
-      <c r="I31" s="43"/>
-      <c r="K31" s="38">
+      <c r="B31" s="43"/>
+      <c r="C31" s="44"/>
+      <c r="H31" s="45"/>
+      <c r="I31" s="46"/>
+      <c r="K31" s="41">
         <v>44684</v>
       </c>
-      <c r="L31" s="39"/>
-      <c r="N31" s="42"/>
-      <c r="O31" s="43"/>
+      <c r="L31" s="42"/>
+      <c r="N31" s="45"/>
+      <c r="O31" s="46"/>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="16">
@@ -1687,18 +1691,18 @@
       <c r="F32" s="34">
         <v>4</v>
       </c>
-      <c r="H32" s="40"/>
-      <c r="I32" s="41"/>
-      <c r="K32" s="42"/>
-      <c r="L32" s="43"/>
-      <c r="N32" s="42"/>
-      <c r="O32" s="43"/>
+      <c r="H32" s="43"/>
+      <c r="I32" s="44"/>
+      <c r="K32" s="45"/>
+      <c r="L32" s="46"/>
+      <c r="N32" s="45"/>
+      <c r="O32" s="46"/>
     </row>
     <row r="33" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="E33" s="38">
+      <c r="E33" s="41">
         <v>44672</v>
       </c>
-      <c r="F33" s="39"/>
+      <c r="F33" s="42"/>
       <c r="G33" s="18">
         <v>6</v>
       </c>
@@ -1709,16 +1713,16 @@
       <c r="I33" s="30">
         <v>4</v>
       </c>
-      <c r="K33" s="42"/>
-      <c r="L33" s="43"/>
-      <c r="N33" s="40"/>
-      <c r="O33" s="41"/>
+      <c r="K33" s="45"/>
+      <c r="L33" s="46"/>
+      <c r="N33" s="43"/>
+      <c r="O33" s="44"/>
     </row>
     <row r="34" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="E34" s="40"/>
-      <c r="F34" s="41"/>
-      <c r="K34" s="42"/>
-      <c r="L34" s="43"/>
+      <c r="E34" s="43"/>
+      <c r="F34" s="44"/>
+      <c r="K34" s="45"/>
+      <c r="L34" s="46"/>
       <c r="M34" s="18"/>
       <c r="N34" s="15" t="str">
         <f>_xlfn.XLOOKUP(Bracket!M34,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
@@ -1737,12 +1741,12 @@
       <c r="F35" s="35">
         <v>1</v>
       </c>
-      <c r="K35" s="42"/>
-      <c r="L35" s="43"/>
+      <c r="K35" s="45"/>
+      <c r="L35" s="46"/>
     </row>
     <row r="36" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="K36" s="42"/>
-      <c r="L36" s="43"/>
+      <c r="K36" s="45"/>
+      <c r="L36" s="46"/>
     </row>
     <row r="37" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D37" s="16">
@@ -1755,14 +1759,14 @@
       <c r="F37" s="34">
         <v>5</v>
       </c>
-      <c r="K37" s="42"/>
-      <c r="L37" s="43"/>
+      <c r="K37" s="45"/>
+      <c r="L37" s="46"/>
     </row>
     <row r="38" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="E38" s="38">
+      <c r="E38" s="41">
         <v>44673</v>
       </c>
-      <c r="F38" s="39"/>
+      <c r="F38" s="42"/>
       <c r="G38" s="18">
         <v>4</v>
       </c>
@@ -1773,18 +1777,18 @@
       <c r="I38" s="34">
         <v>3</v>
       </c>
-      <c r="K38" s="42"/>
-      <c r="L38" s="43"/>
+      <c r="K38" s="45"/>
+      <c r="L38" s="46"/>
     </row>
     <row r="39" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="E39" s="40"/>
-      <c r="F39" s="41"/>
-      <c r="H39" s="38">
+      <c r="E39" s="43"/>
+      <c r="F39" s="44"/>
+      <c r="H39" s="41">
         <v>44680</v>
       </c>
-      <c r="I39" s="39"/>
-      <c r="K39" s="40"/>
-      <c r="L39" s="41"/>
+      <c r="I39" s="42"/>
+      <c r="K39" s="43"/>
+      <c r="L39" s="44"/>
     </row>
     <row r="40" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D40" s="16">
@@ -1797,8 +1801,8 @@
       <c r="F40" s="35">
         <v>1</v>
       </c>
-      <c r="H40" s="42"/>
-      <c r="I40" s="43"/>
+      <c r="H40" s="45"/>
+      <c r="I40" s="46"/>
       <c r="J40" s="18">
         <v>4</v>
       </c>
@@ -1809,8 +1813,8 @@
       <c r="L40" s="28"/>
     </row>
     <row r="41" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="H41" s="42"/>
-      <c r="I41" s="43"/>
+      <c r="H41" s="45"/>
+      <c r="I41" s="46"/>
     </row>
     <row r="42" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D42" s="16">
@@ -1823,14 +1827,14 @@
       <c r="F42" s="37">
         <v>1</v>
       </c>
-      <c r="H42" s="40"/>
-      <c r="I42" s="41"/>
+      <c r="H42" s="43"/>
+      <c r="I42" s="44"/>
     </row>
     <row r="43" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="E43" s="38">
+      <c r="E43" s="41">
         <v>44676</v>
       </c>
-      <c r="F43" s="39"/>
+      <c r="F43" s="42"/>
       <c r="G43" s="18">
         <v>9</v>
       </c>
@@ -1845,8 +1849,8 @@
     <row r="44" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B44" s="9"/>
       <c r="C44" s="9"/>
-      <c r="E44" s="40"/>
-      <c r="F44" s="41"/>
+      <c r="E44" s="43"/>
+      <c r="F44" s="44"/>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45" s="9"/>
@@ -1872,6 +1876,11 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="E43:F44"/>
+    <mergeCell ref="H29:I32"/>
+    <mergeCell ref="H39:I42"/>
+    <mergeCell ref="B30:C31"/>
+    <mergeCell ref="E23:F24"/>
     <mergeCell ref="B2:Q2"/>
     <mergeCell ref="B10:C11"/>
     <mergeCell ref="E8:F9"/>
@@ -1885,11 +1894,6 @@
     <mergeCell ref="E33:F34"/>
     <mergeCell ref="K31:L39"/>
     <mergeCell ref="E38:F39"/>
-    <mergeCell ref="E43:F44"/>
-    <mergeCell ref="H29:I32"/>
-    <mergeCell ref="H39:I42"/>
-    <mergeCell ref="B30:C31"/>
-    <mergeCell ref="E23:F24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Nutty Buddy wins again
</commit_message>
<xml_diff>
--- a/LilDebBracket.xlsx
+++ b/LilDebBracket.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kwiktrip-my.sharepoint.com/personal/am10014003_kwiktrip_com/Documents/Development/lildeb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{6E5F7E92-F189-4DFC-B03F-793BA7D32A3A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{5A6CE12B-4652-44AB-BB0E-1E953A01B951}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{6E5F7E92-F189-4DFC-B03F-793BA7D32A3A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{3F2A3C1F-C0DC-4D90-864B-02A1C986F85A}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{10960CD5-A4F3-447E-9C42-3300723A7601}"/>
+    <workbookView xWindow="38385" yWindow="15900" windowWidth="19215" windowHeight="15900" xr2:uid="{10960CD5-A4F3-447E-9C42-3300723A7601}"/>
   </bookViews>
   <sheets>
     <sheet name="Bracket" sheetId="3" r:id="rId1"/>
@@ -633,15 +633,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="16" fontId="4" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -659,6 +650,15 @@
     </xf>
     <xf numFmtId="16" fontId="4" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1199,24 +1199,24 @@
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:17" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
-      <c r="M2" s="39"/>
-      <c r="N2" s="39"/>
-      <c r="O2" s="39"/>
-      <c r="P2" s="39"/>
-      <c r="Q2" s="40"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="45"/>
+      <c r="L2" s="45"/>
+      <c r="M2" s="45"/>
+      <c r="N2" s="45"/>
+      <c r="O2" s="45"/>
+      <c r="P2" s="45"/>
+      <c r="Q2" s="46"/>
     </row>
     <row r="3" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B3" s="11"/>
@@ -1274,10 +1274,10 @@
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E8" s="41">
+      <c r="E8" s="38">
         <v>44663</v>
       </c>
-      <c r="F8" s="42"/>
+      <c r="F8" s="39"/>
       <c r="G8" s="18">
         <v>17</v>
       </c>
@@ -1300,18 +1300,18 @@
       <c r="C9" s="32">
         <v>2</v>
       </c>
-      <c r="E9" s="43"/>
-      <c r="F9" s="44"/>
-      <c r="H9" s="41">
+      <c r="E9" s="40"/>
+      <c r="F9" s="41"/>
+      <c r="H9" s="38">
         <v>44679</v>
       </c>
-      <c r="I9" s="42"/>
+      <c r="I9" s="39"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B10" s="41">
+      <c r="B10" s="38">
         <v>44662</v>
       </c>
-      <c r="C10" s="42"/>
+      <c r="C10" s="39"/>
       <c r="D10" s="18">
         <v>17</v>
       </c>
@@ -1322,8 +1322,8 @@
       <c r="F10" s="31">
         <v>4</v>
       </c>
-      <c r="H10" s="45"/>
-      <c r="I10" s="46"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="43"/>
       <c r="J10" s="18">
         <v>17</v>
       </c>
@@ -1336,14 +1336,14 @@
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B11" s="43"/>
-      <c r="C11" s="44"/>
-      <c r="H11" s="45"/>
-      <c r="I11" s="46"/>
-      <c r="K11" s="41">
+      <c r="B11" s="40"/>
+      <c r="C11" s="41"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="43"/>
+      <c r="K11" s="38">
         <v>44683</v>
       </c>
-      <c r="L11" s="42"/>
+      <c r="L11" s="39"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="16">
@@ -1366,16 +1366,16 @@
       <c r="F12" s="34">
         <v>3</v>
       </c>
-      <c r="H12" s="43"/>
-      <c r="I12" s="44"/>
-      <c r="K12" s="45"/>
-      <c r="L12" s="46"/>
+      <c r="H12" s="40"/>
+      <c r="I12" s="41"/>
+      <c r="K12" s="42"/>
+      <c r="L12" s="43"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E13" s="41">
+      <c r="E13" s="38">
         <v>44664</v>
       </c>
-      <c r="F13" s="42"/>
+      <c r="F13" s="39"/>
       <c r="G13" s="18">
         <v>3</v>
       </c>
@@ -1386,14 +1386,14 @@
       <c r="I13" s="37">
         <v>0</v>
       </c>
-      <c r="K13" s="45"/>
-      <c r="L13" s="46"/>
+      <c r="K13" s="42"/>
+      <c r="L13" s="43"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E14" s="43"/>
-      <c r="F14" s="44"/>
-      <c r="K14" s="45"/>
-      <c r="L14" s="46"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="41"/>
+      <c r="K14" s="42"/>
+      <c r="L14" s="43"/>
       <c r="M14" s="18">
         <v>17</v>
       </c>
@@ -1414,18 +1414,18 @@
       <c r="F15" s="35">
         <v>2</v>
       </c>
-      <c r="K15" s="45"/>
-      <c r="L15" s="46"/>
-      <c r="N15" s="41">
+      <c r="K15" s="42"/>
+      <c r="L15" s="43"/>
+      <c r="N15" s="38">
         <v>44685</v>
       </c>
-      <c r="O15" s="42"/>
+      <c r="O15" s="39"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="K16" s="45"/>
-      <c r="L16" s="46"/>
-      <c r="N16" s="45"/>
-      <c r="O16" s="46"/>
+      <c r="K16" s="42"/>
+      <c r="L16" s="43"/>
+      <c r="N16" s="42"/>
+      <c r="O16" s="43"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D17" s="16">
@@ -1438,16 +1438,16 @@
       <c r="F17" s="34">
         <v>5</v>
       </c>
-      <c r="K17" s="45"/>
-      <c r="L17" s="46"/>
-      <c r="N17" s="45"/>
-      <c r="O17" s="46"/>
+      <c r="K17" s="42"/>
+      <c r="L17" s="43"/>
+      <c r="N17" s="42"/>
+      <c r="O17" s="43"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E18" s="41">
+      <c r="E18" s="38">
         <v>44665</v>
       </c>
-      <c r="F18" s="42"/>
+      <c r="F18" s="39"/>
       <c r="G18" s="18">
         <v>5</v>
       </c>
@@ -1458,22 +1458,22 @@
       <c r="I18" s="34">
         <v>3</v>
       </c>
-      <c r="K18" s="45"/>
-      <c r="L18" s="46"/>
-      <c r="N18" s="45"/>
-      <c r="O18" s="46"/>
+      <c r="K18" s="42"/>
+      <c r="L18" s="43"/>
+      <c r="N18" s="42"/>
+      <c r="O18" s="43"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E19" s="43"/>
-      <c r="F19" s="44"/>
-      <c r="H19" s="41">
+      <c r="E19" s="40"/>
+      <c r="F19" s="41"/>
+      <c r="H19" s="38">
         <v>44677</v>
       </c>
-      <c r="I19" s="42"/>
-      <c r="K19" s="43"/>
-      <c r="L19" s="44"/>
-      <c r="N19" s="45"/>
-      <c r="O19" s="46"/>
+      <c r="I19" s="39"/>
+      <c r="K19" s="40"/>
+      <c r="L19" s="41"/>
+      <c r="N19" s="42"/>
+      <c r="O19" s="43"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D20" s="16">
@@ -1486,8 +1486,8 @@
       <c r="F20" s="35">
         <v>0</v>
       </c>
-      <c r="H20" s="45"/>
-      <c r="I20" s="46"/>
+      <c r="H20" s="42"/>
+      <c r="I20" s="43"/>
       <c r="J20" s="18">
         <v>5</v>
       </c>
@@ -1498,14 +1498,14 @@
       <c r="L20" s="35">
         <v>2</v>
       </c>
-      <c r="N20" s="45"/>
-      <c r="O20" s="46"/>
+      <c r="N20" s="42"/>
+      <c r="O20" s="43"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="H21" s="45"/>
-      <c r="I21" s="46"/>
-      <c r="N21" s="45"/>
-      <c r="O21" s="46"/>
+      <c r="H21" s="42"/>
+      <c r="I21" s="43"/>
+      <c r="N21" s="42"/>
+      <c r="O21" s="43"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D22" s="16">
@@ -1518,16 +1518,16 @@
       <c r="F22" s="34">
         <v>4</v>
       </c>
-      <c r="H22" s="43"/>
-      <c r="I22" s="44"/>
-      <c r="N22" s="45"/>
-      <c r="O22" s="46"/>
+      <c r="H22" s="40"/>
+      <c r="I22" s="41"/>
+      <c r="N22" s="42"/>
+      <c r="O22" s="43"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E23" s="41">
+      <c r="E23" s="38">
         <v>44669</v>
       </c>
-      <c r="F23" s="42"/>
+      <c r="F23" s="39"/>
       <c r="G23" s="18">
         <v>7</v>
       </c>
@@ -1538,8 +1538,8 @@
       <c r="I23" s="37">
         <v>2</v>
       </c>
-      <c r="N23" s="45"/>
-      <c r="O23" s="46"/>
+      <c r="N23" s="42"/>
+      <c r="O23" s="43"/>
       <c r="P23" s="18"/>
       <c r="Q23" s="15" t="str">
         <f>_xlfn.XLOOKUP(Bracket!P23,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
@@ -1549,10 +1549,10 @@
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
-      <c r="E24" s="43"/>
-      <c r="F24" s="44"/>
-      <c r="N24" s="45"/>
-      <c r="O24" s="46"/>
+      <c r="E24" s="40"/>
+      <c r="F24" s="41"/>
+      <c r="N24" s="42"/>
+      <c r="O24" s="43"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B25" s="9"/>
@@ -1567,14 +1567,14 @@
       <c r="F25" s="35">
         <v>2</v>
       </c>
-      <c r="N25" s="45"/>
-      <c r="O25" s="46"/>
+      <c r="N25" s="42"/>
+      <c r="O25" s="43"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
-      <c r="N26" s="45"/>
-      <c r="O26" s="46"/>
+      <c r="N26" s="42"/>
+      <c r="O26" s="43"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B27" s="9"/>
@@ -1589,14 +1589,14 @@
       <c r="F27" s="32">
         <v>2</v>
       </c>
-      <c r="N27" s="45"/>
-      <c r="O27" s="46"/>
+      <c r="N27" s="42"/>
+      <c r="O27" s="43"/>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E28" s="41">
+      <c r="E28" s="38">
         <v>44671</v>
       </c>
-      <c r="F28" s="42"/>
+      <c r="F28" s="39"/>
       <c r="G28" s="18">
         <v>18</v>
       </c>
@@ -1607,8 +1607,8 @@
       <c r="I28" s="37">
         <v>0</v>
       </c>
-      <c r="N28" s="45"/>
-      <c r="O28" s="46"/>
+      <c r="N28" s="42"/>
+      <c r="O28" s="43"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="16">
@@ -1621,20 +1621,20 @@
       <c r="C29" s="32">
         <v>3</v>
       </c>
-      <c r="E29" s="43"/>
-      <c r="F29" s="44"/>
-      <c r="H29" s="41">
+      <c r="E29" s="40"/>
+      <c r="F29" s="41"/>
+      <c r="H29" s="38">
         <v>44679</v>
       </c>
-      <c r="I29" s="42"/>
-      <c r="N29" s="45"/>
-      <c r="O29" s="46"/>
+      <c r="I29" s="39"/>
+      <c r="N29" s="42"/>
+      <c r="O29" s="43"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B30" s="41">
+      <c r="B30" s="38">
         <v>44670</v>
       </c>
-      <c r="C30" s="42"/>
+      <c r="C30" s="39"/>
       <c r="D30" s="18">
         <v>18</v>
       </c>
@@ -1645,30 +1645,32 @@
       <c r="F30" s="31">
         <v>3</v>
       </c>
-      <c r="H30" s="45"/>
-      <c r="I30" s="46"/>
+      <c r="H30" s="42"/>
+      <c r="I30" s="43"/>
       <c r="J30" s="18">
         <v>6</v>
       </c>
-      <c r="K30" s="15" t="str">
+      <c r="K30" s="33" t="str">
         <f>_xlfn.XLOOKUP(Bracket!J30,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
         <v>Oatmeal Cream Pies</v>
       </c>
-      <c r="L30" s="27"/>
-      <c r="N30" s="45"/>
-      <c r="O30" s="46"/>
+      <c r="L30" s="32">
+        <v>2</v>
+      </c>
+      <c r="N30" s="42"/>
+      <c r="O30" s="43"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B31" s="43"/>
-      <c r="C31" s="44"/>
-      <c r="H31" s="45"/>
-      <c r="I31" s="46"/>
-      <c r="K31" s="41">
+      <c r="B31" s="40"/>
+      <c r="C31" s="41"/>
+      <c r="H31" s="42"/>
+      <c r="I31" s="43"/>
+      <c r="K31" s="38">
         <v>44684</v>
       </c>
-      <c r="L31" s="42"/>
-      <c r="N31" s="45"/>
-      <c r="O31" s="46"/>
+      <c r="L31" s="39"/>
+      <c r="N31" s="42"/>
+      <c r="O31" s="43"/>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="16">
@@ -1691,18 +1693,18 @@
       <c r="F32" s="34">
         <v>4</v>
       </c>
-      <c r="H32" s="43"/>
-      <c r="I32" s="44"/>
-      <c r="K32" s="45"/>
-      <c r="L32" s="46"/>
-      <c r="N32" s="45"/>
-      <c r="O32" s="46"/>
+      <c r="H32" s="40"/>
+      <c r="I32" s="41"/>
+      <c r="K32" s="42"/>
+      <c r="L32" s="43"/>
+      <c r="N32" s="42"/>
+      <c r="O32" s="43"/>
     </row>
     <row r="33" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="E33" s="41">
+      <c r="E33" s="38">
         <v>44672</v>
       </c>
-      <c r="F33" s="42"/>
+      <c r="F33" s="39"/>
       <c r="G33" s="18">
         <v>6</v>
       </c>
@@ -1713,20 +1715,22 @@
       <c r="I33" s="30">
         <v>4</v>
       </c>
-      <c r="K33" s="45"/>
-      <c r="L33" s="46"/>
-      <c r="N33" s="43"/>
-      <c r="O33" s="44"/>
+      <c r="K33" s="42"/>
+      <c r="L33" s="43"/>
+      <c r="N33" s="40"/>
+      <c r="O33" s="41"/>
     </row>
     <row r="34" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="E34" s="43"/>
-      <c r="F34" s="44"/>
-      <c r="K34" s="45"/>
-      <c r="L34" s="46"/>
-      <c r="M34" s="18"/>
+      <c r="E34" s="40"/>
+      <c r="F34" s="41"/>
+      <c r="K34" s="42"/>
+      <c r="L34" s="43"/>
+      <c r="M34" s="18">
+        <v>4</v>
+      </c>
       <c r="N34" s="15" t="str">
         <f>_xlfn.XLOOKUP(Bracket!M34,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
-        <v>TBD</v>
+        <v>Nutty Buddy</v>
       </c>
       <c r="O34" s="28"/>
     </row>
@@ -1741,12 +1745,12 @@
       <c r="F35" s="35">
         <v>1</v>
       </c>
-      <c r="K35" s="45"/>
-      <c r="L35" s="46"/>
+      <c r="K35" s="42"/>
+      <c r="L35" s="43"/>
     </row>
     <row r="36" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="K36" s="45"/>
-      <c r="L36" s="46"/>
+      <c r="K36" s="42"/>
+      <c r="L36" s="43"/>
     </row>
     <row r="37" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D37" s="16">
@@ -1759,14 +1763,14 @@
       <c r="F37" s="34">
         <v>5</v>
       </c>
-      <c r="K37" s="45"/>
-      <c r="L37" s="46"/>
+      <c r="K37" s="42"/>
+      <c r="L37" s="43"/>
     </row>
     <row r="38" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="E38" s="41">
+      <c r="E38" s="38">
         <v>44673</v>
       </c>
-      <c r="F38" s="42"/>
+      <c r="F38" s="39"/>
       <c r="G38" s="18">
         <v>4</v>
       </c>
@@ -1777,18 +1781,18 @@
       <c r="I38" s="34">
         <v>3</v>
       </c>
-      <c r="K38" s="45"/>
-      <c r="L38" s="46"/>
+      <c r="K38" s="42"/>
+      <c r="L38" s="43"/>
     </row>
     <row r="39" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="E39" s="43"/>
-      <c r="F39" s="44"/>
-      <c r="H39" s="41">
+      <c r="E39" s="40"/>
+      <c r="F39" s="41"/>
+      <c r="H39" s="38">
         <v>44680</v>
       </c>
-      <c r="I39" s="42"/>
-      <c r="K39" s="43"/>
-      <c r="L39" s="44"/>
+      <c r="I39" s="39"/>
+      <c r="K39" s="40"/>
+      <c r="L39" s="41"/>
     </row>
     <row r="40" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D40" s="16">
@@ -1801,20 +1805,22 @@
       <c r="F40" s="35">
         <v>1</v>
       </c>
-      <c r="H40" s="45"/>
-      <c r="I40" s="46"/>
+      <c r="H40" s="42"/>
+      <c r="I40" s="43"/>
       <c r="J40" s="18">
         <v>4</v>
       </c>
-      <c r="K40" s="15" t="str">
+      <c r="K40" s="30" t="str">
         <f>_xlfn.XLOOKUP(Bracket!J40,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
         <v>Nutty Buddy</v>
       </c>
-      <c r="L40" s="28"/>
+      <c r="L40" s="31">
+        <v>3</v>
+      </c>
     </row>
     <row r="41" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="H41" s="45"/>
-      <c r="I41" s="46"/>
+      <c r="H41" s="42"/>
+      <c r="I41" s="43"/>
     </row>
     <row r="42" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D42" s="16">
@@ -1827,14 +1833,14 @@
       <c r="F42" s="37">
         <v>1</v>
       </c>
-      <c r="H42" s="43"/>
-      <c r="I42" s="44"/>
+      <c r="H42" s="40"/>
+      <c r="I42" s="41"/>
     </row>
     <row r="43" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="E43" s="41">
+      <c r="E43" s="38">
         <v>44676</v>
       </c>
-      <c r="F43" s="42"/>
+      <c r="F43" s="39"/>
       <c r="G43" s="18">
         <v>9</v>
       </c>
@@ -1849,8 +1855,8 @@
     <row r="44" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B44" s="9"/>
       <c r="C44" s="9"/>
-      <c r="E44" s="43"/>
-      <c r="F44" s="44"/>
+      <c r="E44" s="40"/>
+      <c r="F44" s="41"/>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45" s="9"/>
@@ -1876,11 +1882,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="E43:F44"/>
-    <mergeCell ref="H29:I32"/>
-    <mergeCell ref="H39:I42"/>
-    <mergeCell ref="B30:C31"/>
-    <mergeCell ref="E23:F24"/>
     <mergeCell ref="B2:Q2"/>
     <mergeCell ref="B10:C11"/>
     <mergeCell ref="E8:F9"/>
@@ -1894,6 +1895,11 @@
     <mergeCell ref="E33:F34"/>
     <mergeCell ref="K31:L39"/>
     <mergeCell ref="E38:F39"/>
+    <mergeCell ref="E43:F44"/>
+    <mergeCell ref="H29:I32"/>
+    <mergeCell ref="H39:I42"/>
+    <mergeCell ref="B30:C31"/>
+    <mergeCell ref="E23:F24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated date for finals
</commit_message>
<xml_diff>
--- a/LilDebBracket.xlsx
+++ b/LilDebBracket.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kwiktrip-my.sharepoint.com/personal/am10014003_kwiktrip_com/Documents/Development/lildeb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{6E5F7E92-F189-4DFC-B03F-793BA7D32A3A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{3F2A3C1F-C0DC-4D90-864B-02A1C986F85A}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{6E5F7E92-F189-4DFC-B03F-793BA7D32A3A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B8A9FADB-B2E9-4705-B8D0-4F6DC903A209}"/>
   <bookViews>
-    <workbookView xWindow="38385" yWindow="15900" windowWidth="19215" windowHeight="15900" xr2:uid="{10960CD5-A4F3-447E-9C42-3300723A7601}"/>
+    <workbookView xWindow="4545" yWindow="3855" windowWidth="28800" windowHeight="15435" xr2:uid="{10960CD5-A4F3-447E-9C42-3300723A7601}"/>
   </bookViews>
   <sheets>
     <sheet name="Bracket" sheetId="3" r:id="rId1"/>
@@ -633,6 +633,15 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="16" fontId="4" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -650,15 +659,6 @@
     </xf>
     <xf numFmtId="16" fontId="4" fillId="4" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1178,7 +1178,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0E5BB06-8011-4308-BEC9-9A7436B98035}">
   <dimension ref="A1:Q47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="N34" sqref="N34"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1199,24 +1201,24 @@
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:17" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="45"/>
-      <c r="M2" s="45"/>
-      <c r="N2" s="45"/>
-      <c r="O2" s="45"/>
-      <c r="P2" s="45"/>
-      <c r="Q2" s="46"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
+      <c r="N2" s="39"/>
+      <c r="O2" s="39"/>
+      <c r="P2" s="39"/>
+      <c r="Q2" s="40"/>
     </row>
     <row r="3" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B3" s="11"/>
@@ -1274,10 +1276,10 @@
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E8" s="38">
+      <c r="E8" s="41">
         <v>44663</v>
       </c>
-      <c r="F8" s="39"/>
+      <c r="F8" s="42"/>
       <c r="G8" s="18">
         <v>17</v>
       </c>
@@ -1300,18 +1302,18 @@
       <c r="C9" s="32">
         <v>2</v>
       </c>
-      <c r="E9" s="40"/>
-      <c r="F9" s="41"/>
-      <c r="H9" s="38">
+      <c r="E9" s="43"/>
+      <c r="F9" s="44"/>
+      <c r="H9" s="41">
         <v>44679</v>
       </c>
-      <c r="I9" s="39"/>
+      <c r="I9" s="42"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B10" s="38">
+      <c r="B10" s="41">
         <v>44662</v>
       </c>
-      <c r="C10" s="39"/>
+      <c r="C10" s="42"/>
       <c r="D10" s="18">
         <v>17</v>
       </c>
@@ -1322,8 +1324,8 @@
       <c r="F10" s="31">
         <v>4</v>
       </c>
-      <c r="H10" s="42"/>
-      <c r="I10" s="43"/>
+      <c r="H10" s="45"/>
+      <c r="I10" s="46"/>
       <c r="J10" s="18">
         <v>17</v>
       </c>
@@ -1336,14 +1338,14 @@
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B11" s="40"/>
-      <c r="C11" s="41"/>
-      <c r="H11" s="42"/>
-      <c r="I11" s="43"/>
-      <c r="K11" s="38">
+      <c r="B11" s="43"/>
+      <c r="C11" s="44"/>
+      <c r="H11" s="45"/>
+      <c r="I11" s="46"/>
+      <c r="K11" s="41">
         <v>44683</v>
       </c>
-      <c r="L11" s="39"/>
+      <c r="L11" s="42"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="16">
@@ -1366,16 +1368,16 @@
       <c r="F12" s="34">
         <v>3</v>
       </c>
-      <c r="H12" s="40"/>
-      <c r="I12" s="41"/>
-      <c r="K12" s="42"/>
-      <c r="L12" s="43"/>
+      <c r="H12" s="43"/>
+      <c r="I12" s="44"/>
+      <c r="K12" s="45"/>
+      <c r="L12" s="46"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E13" s="38">
+      <c r="E13" s="41">
         <v>44664</v>
       </c>
-      <c r="F13" s="39"/>
+      <c r="F13" s="42"/>
       <c r="G13" s="18">
         <v>3</v>
       </c>
@@ -1386,14 +1388,14 @@
       <c r="I13" s="37">
         <v>0</v>
       </c>
-      <c r="K13" s="42"/>
-      <c r="L13" s="43"/>
+      <c r="K13" s="45"/>
+      <c r="L13" s="46"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E14" s="40"/>
-      <c r="F14" s="41"/>
-      <c r="K14" s="42"/>
-      <c r="L14" s="43"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="44"/>
+      <c r="K14" s="45"/>
+      <c r="L14" s="46"/>
       <c r="M14" s="18">
         <v>17</v>
       </c>
@@ -1414,18 +1416,18 @@
       <c r="F15" s="35">
         <v>2</v>
       </c>
-      <c r="K15" s="42"/>
-      <c r="L15" s="43"/>
-      <c r="N15" s="38">
-        <v>44685</v>
-      </c>
-      <c r="O15" s="39"/>
+      <c r="K15" s="45"/>
+      <c r="L15" s="46"/>
+      <c r="N15" s="41">
+        <v>44686</v>
+      </c>
+      <c r="O15" s="42"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="K16" s="42"/>
-      <c r="L16" s="43"/>
-      <c r="N16" s="42"/>
-      <c r="O16" s="43"/>
+      <c r="K16" s="45"/>
+      <c r="L16" s="46"/>
+      <c r="N16" s="45"/>
+      <c r="O16" s="46"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D17" s="16">
@@ -1438,16 +1440,16 @@
       <c r="F17" s="34">
         <v>5</v>
       </c>
-      <c r="K17" s="42"/>
-      <c r="L17" s="43"/>
-      <c r="N17" s="42"/>
-      <c r="O17" s="43"/>
+      <c r="K17" s="45"/>
+      <c r="L17" s="46"/>
+      <c r="N17" s="45"/>
+      <c r="O17" s="46"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E18" s="38">
+      <c r="E18" s="41">
         <v>44665</v>
       </c>
-      <c r="F18" s="39"/>
+      <c r="F18" s="42"/>
       <c r="G18" s="18">
         <v>5</v>
       </c>
@@ -1458,22 +1460,22 @@
       <c r="I18" s="34">
         <v>3</v>
       </c>
-      <c r="K18" s="42"/>
-      <c r="L18" s="43"/>
-      <c r="N18" s="42"/>
-      <c r="O18" s="43"/>
+      <c r="K18" s="45"/>
+      <c r="L18" s="46"/>
+      <c r="N18" s="45"/>
+      <c r="O18" s="46"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E19" s="40"/>
-      <c r="F19" s="41"/>
-      <c r="H19" s="38">
+      <c r="E19" s="43"/>
+      <c r="F19" s="44"/>
+      <c r="H19" s="41">
         <v>44677</v>
       </c>
-      <c r="I19" s="39"/>
-      <c r="K19" s="40"/>
-      <c r="L19" s="41"/>
-      <c r="N19" s="42"/>
-      <c r="O19" s="43"/>
+      <c r="I19" s="42"/>
+      <c r="K19" s="43"/>
+      <c r="L19" s="44"/>
+      <c r="N19" s="45"/>
+      <c r="O19" s="46"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D20" s="16">
@@ -1486,8 +1488,8 @@
       <c r="F20" s="35">
         <v>0</v>
       </c>
-      <c r="H20" s="42"/>
-      <c r="I20" s="43"/>
+      <c r="H20" s="45"/>
+      <c r="I20" s="46"/>
       <c r="J20" s="18">
         <v>5</v>
       </c>
@@ -1498,14 +1500,14 @@
       <c r="L20" s="35">
         <v>2</v>
       </c>
-      <c r="N20" s="42"/>
-      <c r="O20" s="43"/>
+      <c r="N20" s="45"/>
+      <c r="O20" s="46"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="H21" s="42"/>
-      <c r="I21" s="43"/>
-      <c r="N21" s="42"/>
-      <c r="O21" s="43"/>
+      <c r="H21" s="45"/>
+      <c r="I21" s="46"/>
+      <c r="N21" s="45"/>
+      <c r="O21" s="46"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D22" s="16">
@@ -1518,16 +1520,16 @@
       <c r="F22" s="34">
         <v>4</v>
       </c>
-      <c r="H22" s="40"/>
-      <c r="I22" s="41"/>
-      <c r="N22" s="42"/>
-      <c r="O22" s="43"/>
+      <c r="H22" s="43"/>
+      <c r="I22" s="44"/>
+      <c r="N22" s="45"/>
+      <c r="O22" s="46"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E23" s="38">
+      <c r="E23" s="41">
         <v>44669</v>
       </c>
-      <c r="F23" s="39"/>
+      <c r="F23" s="42"/>
       <c r="G23" s="18">
         <v>7</v>
       </c>
@@ -1538,8 +1540,8 @@
       <c r="I23" s="37">
         <v>2</v>
       </c>
-      <c r="N23" s="42"/>
-      <c r="O23" s="43"/>
+      <c r="N23" s="45"/>
+      <c r="O23" s="46"/>
       <c r="P23" s="18"/>
       <c r="Q23" s="15" t="str">
         <f>_xlfn.XLOOKUP(Bracket!P23,Competitors!$I$2:$I$19,Competitors!$A$2:$A$19,"TBD",0)</f>
@@ -1549,10 +1551,10 @@
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
-      <c r="E24" s="40"/>
-      <c r="F24" s="41"/>
-      <c r="N24" s="42"/>
-      <c r="O24" s="43"/>
+      <c r="E24" s="43"/>
+      <c r="F24" s="44"/>
+      <c r="N24" s="45"/>
+      <c r="O24" s="46"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B25" s="9"/>
@@ -1567,14 +1569,14 @@
       <c r="F25" s="35">
         <v>2</v>
       </c>
-      <c r="N25" s="42"/>
-      <c r="O25" s="43"/>
+      <c r="N25" s="45"/>
+      <c r="O25" s="46"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
-      <c r="N26" s="42"/>
-      <c r="O26" s="43"/>
+      <c r="N26" s="45"/>
+      <c r="O26" s="46"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B27" s="9"/>
@@ -1589,14 +1591,14 @@
       <c r="F27" s="32">
         <v>2</v>
       </c>
-      <c r="N27" s="42"/>
-      <c r="O27" s="43"/>
+      <c r="N27" s="45"/>
+      <c r="O27" s="46"/>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="E28" s="38">
+      <c r="E28" s="41">
         <v>44671</v>
       </c>
-      <c r="F28" s="39"/>
+      <c r="F28" s="42"/>
       <c r="G28" s="18">
         <v>18</v>
       </c>
@@ -1607,8 +1609,8 @@
       <c r="I28" s="37">
         <v>0</v>
       </c>
-      <c r="N28" s="42"/>
-      <c r="O28" s="43"/>
+      <c r="N28" s="45"/>
+      <c r="O28" s="46"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="16">
@@ -1621,20 +1623,20 @@
       <c r="C29" s="32">
         <v>3</v>
       </c>
-      <c r="E29" s="40"/>
-      <c r="F29" s="41"/>
-      <c r="H29" s="38">
+      <c r="E29" s="43"/>
+      <c r="F29" s="44"/>
+      <c r="H29" s="41">
         <v>44679</v>
       </c>
-      <c r="I29" s="39"/>
-      <c r="N29" s="42"/>
-      <c r="O29" s="43"/>
+      <c r="I29" s="42"/>
+      <c r="N29" s="45"/>
+      <c r="O29" s="46"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B30" s="38">
+      <c r="B30" s="41">
         <v>44670</v>
       </c>
-      <c r="C30" s="39"/>
+      <c r="C30" s="42"/>
       <c r="D30" s="18">
         <v>18</v>
       </c>
@@ -1645,8 +1647,8 @@
       <c r="F30" s="31">
         <v>3</v>
       </c>
-      <c r="H30" s="42"/>
-      <c r="I30" s="43"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="46"/>
       <c r="J30" s="18">
         <v>6</v>
       </c>
@@ -1657,20 +1659,20 @@
       <c r="L30" s="32">
         <v>2</v>
       </c>
-      <c r="N30" s="42"/>
-      <c r="O30" s="43"/>
+      <c r="N30" s="45"/>
+      <c r="O30" s="46"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B31" s="40"/>
-      <c r="C31" s="41"/>
-      <c r="H31" s="42"/>
-      <c r="I31" s="43"/>
-      <c r="K31" s="38">
+      <c r="B31" s="43"/>
+      <c r="C31" s="44"/>
+      <c r="H31" s="45"/>
+      <c r="I31" s="46"/>
+      <c r="K31" s="41">
         <v>44684</v>
       </c>
-      <c r="L31" s="39"/>
-      <c r="N31" s="42"/>
-      <c r="O31" s="43"/>
+      <c r="L31" s="42"/>
+      <c r="N31" s="45"/>
+      <c r="O31" s="46"/>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="16">
@@ -1693,18 +1695,18 @@
       <c r="F32" s="34">
         <v>4</v>
       </c>
-      <c r="H32" s="40"/>
-      <c r="I32" s="41"/>
-      <c r="K32" s="42"/>
-      <c r="L32" s="43"/>
-      <c r="N32" s="42"/>
-      <c r="O32" s="43"/>
+      <c r="H32" s="43"/>
+      <c r="I32" s="44"/>
+      <c r="K32" s="45"/>
+      <c r="L32" s="46"/>
+      <c r="N32" s="45"/>
+      <c r="O32" s="46"/>
     </row>
     <row r="33" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="E33" s="38">
+      <c r="E33" s="41">
         <v>44672</v>
       </c>
-      <c r="F33" s="39"/>
+      <c r="F33" s="42"/>
       <c r="G33" s="18">
         <v>6</v>
       </c>
@@ -1715,16 +1717,16 @@
       <c r="I33" s="30">
         <v>4</v>
       </c>
-      <c r="K33" s="42"/>
-      <c r="L33" s="43"/>
-      <c r="N33" s="40"/>
-      <c r="O33" s="41"/>
+      <c r="K33" s="45"/>
+      <c r="L33" s="46"/>
+      <c r="N33" s="43"/>
+      <c r="O33" s="44"/>
     </row>
     <row r="34" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="E34" s="40"/>
-      <c r="F34" s="41"/>
-      <c r="K34" s="42"/>
-      <c r="L34" s="43"/>
+      <c r="E34" s="43"/>
+      <c r="F34" s="44"/>
+      <c r="K34" s="45"/>
+      <c r="L34" s="46"/>
       <c r="M34" s="18">
         <v>4</v>
       </c>
@@ -1745,12 +1747,12 @@
       <c r="F35" s="35">
         <v>1</v>
       </c>
-      <c r="K35" s="42"/>
-      <c r="L35" s="43"/>
+      <c r="K35" s="45"/>
+      <c r="L35" s="46"/>
     </row>
     <row r="36" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="K36" s="42"/>
-      <c r="L36" s="43"/>
+      <c r="K36" s="45"/>
+      <c r="L36" s="46"/>
     </row>
     <row r="37" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D37" s="16">
@@ -1763,14 +1765,14 @@
       <c r="F37" s="34">
         <v>5</v>
       </c>
-      <c r="K37" s="42"/>
-      <c r="L37" s="43"/>
+      <c r="K37" s="45"/>
+      <c r="L37" s="46"/>
     </row>
     <row r="38" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="E38" s="38">
+      <c r="E38" s="41">
         <v>44673</v>
       </c>
-      <c r="F38" s="39"/>
+      <c r="F38" s="42"/>
       <c r="G38" s="18">
         <v>4</v>
       </c>
@@ -1781,18 +1783,18 @@
       <c r="I38" s="34">
         <v>3</v>
       </c>
-      <c r="K38" s="42"/>
-      <c r="L38" s="43"/>
+      <c r="K38" s="45"/>
+      <c r="L38" s="46"/>
     </row>
     <row r="39" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="E39" s="40"/>
-      <c r="F39" s="41"/>
-      <c r="H39" s="38">
+      <c r="E39" s="43"/>
+      <c r="F39" s="44"/>
+      <c r="H39" s="41">
         <v>44680</v>
       </c>
-      <c r="I39" s="39"/>
-      <c r="K39" s="40"/>
-      <c r="L39" s="41"/>
+      <c r="I39" s="42"/>
+      <c r="K39" s="43"/>
+      <c r="L39" s="44"/>
     </row>
     <row r="40" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D40" s="16">
@@ -1805,8 +1807,8 @@
       <c r="F40" s="35">
         <v>1</v>
       </c>
-      <c r="H40" s="42"/>
-      <c r="I40" s="43"/>
+      <c r="H40" s="45"/>
+      <c r="I40" s="46"/>
       <c r="J40" s="18">
         <v>4</v>
       </c>
@@ -1819,8 +1821,8 @@
       </c>
     </row>
     <row r="41" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="H41" s="42"/>
-      <c r="I41" s="43"/>
+      <c r="H41" s="45"/>
+      <c r="I41" s="46"/>
     </row>
     <row r="42" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D42" s="16">
@@ -1833,14 +1835,14 @@
       <c r="F42" s="37">
         <v>1</v>
       </c>
-      <c r="H42" s="40"/>
-      <c r="I42" s="41"/>
+      <c r="H42" s="43"/>
+      <c r="I42" s="44"/>
     </row>
     <row r="43" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="E43" s="38">
+      <c r="E43" s="41">
         <v>44676</v>
       </c>
-      <c r="F43" s="39"/>
+      <c r="F43" s="42"/>
       <c r="G43" s="18">
         <v>9</v>
       </c>
@@ -1855,8 +1857,8 @@
     <row r="44" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B44" s="9"/>
       <c r="C44" s="9"/>
-      <c r="E44" s="40"/>
-      <c r="F44" s="41"/>
+      <c r="E44" s="43"/>
+      <c r="F44" s="44"/>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45" s="9"/>
@@ -1882,6 +1884,11 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="E43:F44"/>
+    <mergeCell ref="H29:I32"/>
+    <mergeCell ref="H39:I42"/>
+    <mergeCell ref="B30:C31"/>
+    <mergeCell ref="E23:F24"/>
     <mergeCell ref="B2:Q2"/>
     <mergeCell ref="B10:C11"/>
     <mergeCell ref="E8:F9"/>
@@ -1895,11 +1902,6 @@
     <mergeCell ref="E33:F34"/>
     <mergeCell ref="K31:L39"/>
     <mergeCell ref="E38:F39"/>
-    <mergeCell ref="E43:F44"/>
-    <mergeCell ref="H29:I32"/>
-    <mergeCell ref="H39:I42"/>
-    <mergeCell ref="B30:C31"/>
-    <mergeCell ref="E23:F24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>